<commit_message>
Added more translations and code
Some translations have been fixed and we have added the necessary code to generate the log in the format of notebook of python.
</commit_message>
<xml_diff>
--- a/OperationCoding.xlsx
+++ b/OperationCoding.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uses0.sharepoint.com/sites/PEJUS685/Documentos compartidos/General/BPI Challenge/Artículo/Material suplementario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7909D8E-4EE6-4C99-A3C0-6D0DF1FE3712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{F7909D8E-4EE6-4C99-A3C0-6D0DF1FE3712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A453549-5E37-4E13-8929-AD0D5CF95B4D}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="16815" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="915" yWindow="915" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="336">
   <si>
     <t>General operations</t>
   </si>
@@ -57,6 +57,9 @@
     <t>Group activities of logs</t>
   </si>
   <si>
+    <t>It consists of grouping activities from different logs that belong to the same sub process</t>
+  </si>
+  <si>
     <t>Group activities by cycle time</t>
   </si>
   <si>
@@ -69,6 +72,9 @@
     <t>It consists of grouping activities according to the sub-processes to which they belong. </t>
   </si>
   <si>
+    <t>Group activities by role</t>
+  </si>
+  <si>
     <t>It consists of obtaining a subset of activities related to a specific role. </t>
   </si>
   <si>
@@ -96,6 +102,10 @@
     <t>It consists of grouping activities depending on the dates on which they are carried out</t>
   </si>
   <si>
+    <t>A7 Q4 2020:
+Group of activities by years</t>
+  </si>
+  <si>
     <t>Group events by time</t>
   </si>
   <si>
@@ -120,6 +130,10 @@
     <t>It consists of creating more than one subset of traces based on the repetition of activities</t>
   </si>
   <si>
+    <t>A15 Q2 BPI 2019:
+Group of traces depending on the repetition of activities.</t>
+  </si>
+  <si>
     <t>Group traces by activities</t>
   </si>
   <si>
@@ -180,7 +194,13 @@
     <t>It consists of making various calculations in relation to Cycle Time, with respect to different number of events.</t>
   </si>
   <si>
+    <t>Apply decision trees</t>
+  </si>
+  <si>
     <t>It consists of applying the technique of decision-making trees on trace subsets.</t>
+  </si>
+  <si>
+    <t>Apply machine learning techniques</t>
   </si>
   <si>
     <t>It consists of using some Machine Learning technique, such as by ejmeplo linear regression.</t>
@@ -348,6 +368,9 @@
   </si>
   <si>
     <t>Calculate frequency of sub-processes</t>
+  </si>
+  <si>
+    <t>It consists of determining how many times a series of sub processes are carried out. </t>
   </si>
   <si>
     <t>Calculate frequency of traces</t>
@@ -437,6 +460,9 @@
     <t>Calculate number of sub-processes</t>
   </si>
   <si>
+    <t>It consists of performing a count of previously identified sub processes</t>
+  </si>
+  <si>
     <t xml:space="preserve">A3 P5 2015
 Obtención del nº de etapas en las que participan los recursos que realizan las actividades ‘NOCODE Activity’ </t>
   </si>
@@ -503,6 +529,12 @@
     <t>It consists of calculating the percentage of time that resources or events are involved ... etc</t>
   </si>
   <si>
+    <t>Calculate dates of the development of activities of resources</t>
+  </si>
+  <si>
+    <t>It consist of determining in which dates the resources did the activities</t>
+  </si>
+  <si>
     <t>Calculate processing time</t>
   </si>
   <si>
@@ -585,9 +617,6 @@
     <t>It consists of obtaining a subset of activities associated with a specific resource. </t>
   </si>
   <si>
-    <t>Filter activities by rol</t>
-  </si>
-  <si>
     <t>Consiste en obtener un subconjunto de actividades llevadas a cabo por un rol específico </t>
   </si>
   <si>
@@ -689,9 +718,6 @@
     <t>It consists of obtaining a subset of traces that meet some condition regarding cycle time. </t>
   </si>
   <si>
-    <t>Filter traces by rol</t>
-  </si>
-  <si>
     <t>It consists of obtaining a subset of traces in which a specific role is or is not involved. </t>
   </si>
   <si>
@@ -716,6 +742,9 @@
     <t>Identify sub-processes as bottlenecks applying temporal performance criteria</t>
   </si>
   <si>
+    <t>It consists of detecting which subprocesses have a higher cycle time, or a higher average cycle time, ... etc; either calculating some type of measurements or making a graph.</t>
+  </si>
+  <si>
     <t>Identify activities as bottlenecks applying temporal performance criteria and statistical measures</t>
   </si>
   <si>
@@ -735,6 +764,9 @@
   </si>
   <si>
     <t>Identify sub-processes with incorrect orders with respect to the happy path as bottlenecks</t>
+  </si>
+  <si>
+    <t>It consists of determining subprocesses that have incorrect activity orders with respect to the happy path</t>
   </si>
   <si>
     <t>Identify impact of bottlenecks by organizational unit</t>
@@ -811,9 +843,6 @@
   <si>
     <t>A7 P1 2015
 Consideracion de los recursos identificados como ‘personas involucradas en más de una etapa del proceso’.</t>
-  </si>
-  <si>
-    <t>Identify rol associated with bottlenecks</t>
   </si>
   <si>
     <t>It consists of identifying roles depending on the cycle time they need to carry out activities</t>
@@ -1033,36 +1062,13 @@
     <t>It consists of representing the measurement of a characteristic of subprocesses / activities (Y axis) over time (X axis) to show its trend.For example, the embodiment of a subprocess (0: is not performed, 1: performed) can be represented as a time series.</t>
   </si>
   <si>
-    <t>It consists of grouping activities from different logs that belong to the same sub process</t>
-  </si>
-  <si>
-    <t>Group activities by role</t>
-  </si>
-  <si>
-    <t>It consists of determining how many times a series of sub processes are carried out. </t>
-  </si>
-  <si>
-    <t>It consists of performing a count of previously identified sub processes</t>
-  </si>
-  <si>
-    <t>It consists of detecting which subprocesses have a higher cycle time, or a higher average cycle time, ... etc; either calculating some type of measurements or making a graph.</t>
-  </si>
-  <si>
-    <t>It consists of determining subprocesses that have incorrect activity orders with respect to the happy path</t>
-  </si>
-  <si>
-    <t>A15 Q2 BPI 2019:
-Group of traces depending on the repetition of activities.</t>
-  </si>
-  <si>
-    <t>A7 Q4 2020:
-Group of activities by years</t>
-  </si>
-  <si>
-    <t>Apply decision trees</t>
-  </si>
-  <si>
-    <t>Apply machine learning techniques</t>
+    <t>Filter activities by role</t>
+  </si>
+  <si>
+    <t>Filter traces by role</t>
+  </si>
+  <si>
+    <t>Identify role associated with bottlenecks</t>
   </si>
 </sst>
 </file>
@@ -1130,13 +1136,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1488,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,17 +1533,17 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>324</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1542,13 +1551,13 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1556,13 +1565,13 @@
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1570,13 +1579,13 @@
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
-        <v>325</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1584,13 +1593,13 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1598,13 +1607,13 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1612,13 +1621,13 @@
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1626,16 +1635,16 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>331</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1643,10 +1652,10 @@
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1656,17 +1665,17 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>24</v>
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1674,29 +1683,29 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>330</v>
+        <v>32</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1704,13 +1713,13 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1718,13 +1727,13 @@
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -1732,13 +1741,13 @@
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
       <c r="C16" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1746,13 +1755,13 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1760,13 +1769,13 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1774,13 +1783,13 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1788,13 +1797,13 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1803,10 +1812,10 @@
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1817,10 +1826,10 @@
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -1831,10 +1840,10 @@
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>332</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -1845,10 +1854,10 @@
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>333</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1859,10 +1868,10 @@
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1872,17 +1881,17 @@
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>54</v>
+      <c r="A26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1890,10 +1899,10 @@
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1902,13 +1911,13 @@
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1916,13 +1925,13 @@
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -1930,13 +1939,13 @@
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1944,13 +1953,13 @@
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1958,13 +1967,13 @@
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1972,13 +1981,13 @@
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1986,13 +1995,13 @@
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
       <c r="C34" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -2000,13 +2009,13 @@
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -2014,13 +2023,13 @@
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
       <c r="C36" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -2028,13 +2037,13 @@
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2042,13 +2051,13 @@
       <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
       <c r="C38" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2056,17 +2065,17 @@
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>81</v>
+      <c r="A39" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2074,13 +2083,13 @@
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="4"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
       <c r="C40" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2088,13 +2097,13 @@
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
       <c r="C41" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2102,33 +2111,33 @@
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
       <c r="C42" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>92</v>
+      <c r="A43" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2136,29 +2145,29 @@
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="6"/>
       <c r="C44" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="5"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="6"/>
       <c r="C45" s="1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2166,13 +2175,13 @@
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="5"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="6"/>
       <c r="C46" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -2180,13 +2189,13 @@
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="5"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="6"/>
       <c r="C47" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2194,13 +2203,13 @@
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="5"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="6"/>
       <c r="C48" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>326</v>
+        <v>111</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2208,13 +2217,13 @@
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="5"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="6"/>
       <c r="C49" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2222,32 +2231,32 @@
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="5"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="6"/>
       <c r="C50" s="1" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="5"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="6"/>
       <c r="C51" s="1" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2255,10 +2264,10 @@
     </row>
     <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -2268,49 +2277,49 @@
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>116</v>
+      <c r="A53" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
       <c r="C54" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
       <c r="C55" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2318,26 +2327,26 @@
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
       <c r="C56" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="5"/>
       <c r="C57" s="1" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2346,13 +2355,13 @@
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="4"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
       <c r="C58" s="1" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -2360,65 +2369,65 @@
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
       <c r="C59" s="1" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>327</v>
+        <v>139</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
       <c r="C60" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
       <c r="C61" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>140</v>
+      <c r="A62" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -2426,13 +2435,13 @@
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="5"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="6"/>
       <c r="C63" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -2440,13 +2449,13 @@
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="5"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="6"/>
       <c r="C64" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -2454,13 +2463,13 @@
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="5"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="6"/>
       <c r="C65" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -2468,13 +2477,13 @@
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="5"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="6"/>
       <c r="C66" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -2482,25 +2491,25 @@
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="5"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="6"/>
       <c r="C67" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>154</v>
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -2509,12 +2518,12 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -2523,12 +2532,12 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -2537,42 +2546,42 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="1" t="s">
-        <v>161</v>
-      </c>
+      <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
+      <c r="E72" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -2581,12 +2590,12 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
     </row>
-    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
@@ -2597,10 +2606,10 @@
     </row>
     <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
@@ -2609,12 +2618,12 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
     </row>
-    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2623,12 +2632,12 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -2637,170 +2646,170 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
     </row>
-    <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>177</v>
-      </c>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="4"/>
+      <c r="A79" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>185</v>
+      </c>
       <c r="C79" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
     </row>
-    <row r="80" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
+    <row r="80" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
       <c r="C80" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
     </row>
-    <row r="81" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="4"/>
+    <row r="81" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A81" s="5"/>
+      <c r="B81" s="5"/>
       <c r="C81" s="1" t="s">
-        <v>182</v>
+        <v>333</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
     </row>
-    <row r="82" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
+    <row r="82" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
       <c r="C82" s="1" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>186</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
     </row>
-    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
+    <row r="83" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>195</v>
+      </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>192</v>
-      </c>
+      <c r="A84" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
     </row>
-    <row r="85" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A85" s="4"/>
-      <c r="B85" s="4"/>
+    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>199</v>
+      </c>
       <c r="C85" s="1" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>195</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
     </row>
-    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
+    <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
       <c r="C86" s="1" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E86" s="1"/>
+        <v>203</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
     </row>
     <row r="87" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>199</v>
-      </c>
+      <c r="A87" s="5"/>
+      <c r="B87" s="5"/>
       <c r="C87" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
     </row>
-    <row r="88" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
+    <row r="88" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="C88" s="1" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -2808,27 +2817,27 @@
       <c r="H88" s="1"/>
     </row>
     <row r="89" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
       <c r="C89" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
     </row>
-    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
+    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="5"/>
+      <c r="B90" s="5"/>
       <c r="C90" s="1" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -2836,13 +2845,13 @@
       <c r="H90" s="1"/>
     </row>
     <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-      <c r="B91" s="4"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
       <c r="C91" s="1" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -2850,13 +2859,13 @@
       <c r="H91" s="1"/>
     </row>
     <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
       <c r="C92" s="1" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -2864,13 +2873,13 @@
       <c r="H92" s="1"/>
     </row>
     <row r="93" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="4"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="5"/>
       <c r="C93" s="1" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -2878,322 +2887,320 @@
       <c r="H93" s="1"/>
     </row>
     <row r="94" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
       <c r="C94" s="1" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
+    <row r="95" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
       <c r="C95" s="1" t="s">
-        <v>216</v>
+        <v>334</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
     </row>
-    <row r="96" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>219</v>
-      </c>
+    <row r="96" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="5"/>
+      <c r="B96" s="5"/>
       <c r="C96" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
+    <row r="97" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="C97" s="1" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>328</v>
+        <v>229</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="4"/>
-      <c r="C98" s="3" t="s">
-        <v>223</v>
+    <row r="98" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="1" t="s">
+        <v>230</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
     </row>
-    <row r="99" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="1" t="s">
-        <v>225</v>
+    <row r="99" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5"/>
+      <c r="C99" s="4" t="s">
+        <v>232</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
     </row>
-    <row r="100" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A100" s="4"/>
-      <c r="B100" s="4"/>
+    <row r="100" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
       <c r="C100" s="1" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
     </row>
-    <row r="101" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="4"/>
+    <row r="101" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
       <c r="C101" s="1" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>329</v>
+        <v>237</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
     </row>
-    <row r="102" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
+    <row r="102" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="5"/>
+      <c r="B102" s="5"/>
+      <c r="C102" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
     </row>
-    <row r="103" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E103" s="1" t="s">
-        <v>236</v>
-      </c>
+    <row r="103" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
     </row>
     <row r="104" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4"/>
+      <c r="A104" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>243</v>
+      </c>
       <c r="C104" s="1" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E104" s="1"/>
+        <v>245</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
     </row>
     <row r="105" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="4"/>
+      <c r="A105" s="5"/>
+      <c r="B105" s="5"/>
       <c r="C105" s="1" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
     </row>
-    <row r="106" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
-      <c r="B106" s="4"/>
+    <row r="106" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="5"/>
+      <c r="B106" s="5"/>
       <c r="C106" s="1" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>243</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
     </row>
-    <row r="107" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>245</v>
-      </c>
+    <row r="107" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
+      <c r="B107" s="5"/>
       <c r="C107" s="1" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E107" s="1"/>
+        <v>252</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
     </row>
     <row r="108" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
+      <c r="A108" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>255</v>
+      </c>
       <c r="C108" s="1" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="E108" s="1" t="s">
-        <v>250</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
     </row>
     <row r="109" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
+      <c r="A109" s="5"/>
+      <c r="B109" s="5"/>
       <c r="C109" s="1" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
     </row>
     <row r="110" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
+      <c r="A110" s="5"/>
+      <c r="B110" s="5"/>
       <c r="C110" s="1" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
     </row>
     <row r="111" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4"/>
+      <c r="A111" s="5"/>
+      <c r="B111" s="5"/>
       <c r="C111" s="1" t="s">
-        <v>257</v>
+        <v>335</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E111" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
     </row>
-    <row r="112" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1" t="s">
-        <v>261</v>
-      </c>
+    <row r="112" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+      <c r="B112" s="5"/>
+      <c r="C112" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
     </row>
-    <row r="113" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
     </row>
-    <row r="114" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
@@ -3201,102 +3208,104 @@
     </row>
     <row r="115" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
+      <c r="E115" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
-      <c r="E116" s="1" t="s">
-        <v>272</v>
-      </c>
+      <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
     </row>
-    <row r="117" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
+      <c r="E117" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
     </row>
     <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A118" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>278</v>
-      </c>
+      <c r="A118" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A119" s="4"/>
-      <c r="B119" s="4"/>
+    <row r="119" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A119" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>285</v>
+      </c>
       <c r="C119" s="1" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
     </row>
-    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A120" s="4"/>
-      <c r="B120" s="4"/>
+    <row r="120" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A120" s="5"/>
+      <c r="B120" s="5"/>
       <c r="C120" s="1" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
     </row>
-    <row r="121" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
+    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
+      <c r="B121" s="5"/>
       <c r="C121" s="1" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
@@ -3304,63 +3313,63 @@
       <c r="H121" s="1"/>
     </row>
     <row r="122" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A122" s="4"/>
-      <c r="B122" s="4"/>
+      <c r="A122" s="5"/>
+      <c r="B122" s="5"/>
       <c r="C122" s="1" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>287</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
+    <row r="123" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="5"/>
+      <c r="B123" s="5"/>
+      <c r="C123" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="E123" s="1" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
     </row>
-    <row r="124" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A124" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="E124" s="1"/>
+    <row r="124" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
     </row>
-    <row r="125" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="4"/>
-      <c r="B125" s="4"/>
+    <row r="125" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>301</v>
+      </c>
       <c r="C125" s="1" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
@@ -3368,13 +3377,13 @@
       <c r="H125" s="1"/>
     </row>
     <row r="126" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A126" s="4"/>
-      <c r="B126" s="4"/>
+      <c r="A126" s="5"/>
+      <c r="B126" s="5"/>
       <c r="C126" s="1" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
@@ -3382,13 +3391,13 @@
       <c r="H126" s="1"/>
     </row>
     <row r="127" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A127" s="4"/>
-      <c r="B127" s="4"/>
+      <c r="A127" s="5"/>
+      <c r="B127" s="5"/>
       <c r="C127" s="1" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
@@ -3396,13 +3405,13 @@
       <c r="H127" s="1"/>
     </row>
     <row r="128" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A128" s="4"/>
-      <c r="B128" s="4"/>
+      <c r="A128" s="5"/>
+      <c r="B128" s="5"/>
       <c r="C128" s="1" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
@@ -3410,13 +3419,13 @@
       <c r="H128" s="1"/>
     </row>
     <row r="129" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A129" s="4"/>
-      <c r="B129" s="4"/>
+      <c r="A129" s="5"/>
+      <c r="B129" s="5"/>
       <c r="C129" s="1" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
@@ -3424,13 +3433,13 @@
       <c r="H129" s="1"/>
     </row>
     <row r="130" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A130" s="4"/>
-      <c r="B130" s="4"/>
+      <c r="A130" s="5"/>
+      <c r="B130" s="5"/>
       <c r="C130" s="1" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
@@ -3438,89 +3447,89 @@
       <c r="H130" s="1"/>
     </row>
     <row r="131" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="C131" s="1"/>
-      <c r="D131" s="1"/>
-      <c r="E131" s="1" t="s">
-        <v>309</v>
-      </c>
+      <c r="A131" s="5"/>
+      <c r="B131" s="5"/>
+      <c r="C131" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
     <row r="132" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>310</v>
+        <v>316</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
-    <row r="133" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="E133" s="1"/>
+    <row r="133" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
     </row>
-    <row r="134" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A134" s="4"/>
-      <c r="B134" s="4"/>
+    <row r="134" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>323</v>
+      </c>
       <c r="C134" s="1" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A135" s="4"/>
-      <c r="B135" s="4"/>
+    <row r="135" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A135" s="5"/>
+      <c r="B135" s="5"/>
       <c r="C135" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="D135" s="1"/>
+        <v>326</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
-    <row r="136" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C136" s="1"/>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A136" s="5"/>
+      <c r="B136" s="5"/>
+      <c r="C136" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
@@ -3529,10 +3538,10 @@
     </row>
     <row r="137" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -3540,6 +3549,20 @@
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
+    </row>
+    <row r="138" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="1"/>
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="32">
@@ -3557,30 +3580,45 @@
     <mergeCell ref="B53:B61"/>
     <mergeCell ref="A62:A67"/>
     <mergeCell ref="B62:B67"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="A84:A86"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="A87:A95"/>
-    <mergeCell ref="B87:B95"/>
-    <mergeCell ref="A96:A101"/>
-    <mergeCell ref="B96:B101"/>
-    <mergeCell ref="A103:A106"/>
-    <mergeCell ref="B103:B106"/>
-    <mergeCell ref="A107:A111"/>
-    <mergeCell ref="B107:B111"/>
-    <mergeCell ref="A118:A122"/>
-    <mergeCell ref="B118:B122"/>
-    <mergeCell ref="A124:A130"/>
-    <mergeCell ref="B124:B130"/>
-    <mergeCell ref="A133:A135"/>
-    <mergeCell ref="B133:B135"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="B85:B87"/>
+    <mergeCell ref="A88:A96"/>
+    <mergeCell ref="B88:B96"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="B97:B102"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="A108:A112"/>
+    <mergeCell ref="B108:B112"/>
+    <mergeCell ref="A119:A123"/>
+    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="A125:A131"/>
+    <mergeCell ref="B125:B131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -3764,22 +3802,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5280F00-08C5-4424-8C69-5F59D5F29D10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3795,28 +3842,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated coding and logs
Identify bottlenecks has been changed for Find bottlenecks in order to avoid missunderstandings with other operations. This change has been applied for its variants also, therefore it was necessary to reconstruct the log. In addtion, logs with variants as concept name have been moved.
</commit_message>
<xml_diff>
--- a/OperationCoding.xlsx
+++ b/OperationCoding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499CC939-6BD2-4EFD-A28B-9BBD57574C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9712D6-B1B6-4130-96D7-A993C683A353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-630" yWindow="255" windowWidth="22800" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -596,37 +596,19 @@
     <t>It consists of obtaining a subset of traces that meet some condition regarding cycle time. </t>
   </si>
   <si>
-    <t>Identify bottlenecks</t>
-  </si>
-  <si>
     <t>It consists of detecting events, resources, roles or patterns of activities, which suppose arrears or irregularities in the process.</t>
   </si>
   <si>
-    <t>Identify activities as bottlenecks applying temporal performance criteria</t>
-  </si>
-  <si>
     <t>It consists of detecting which activities have a greater cycle time, or a greater average cycle time, or increase the average cycle time of the variants more ... etc; either calculating some type of measurements or making a graph. </t>
   </si>
   <si>
-    <t>Identify sub-processes as bottlenecks applying temporal performance criteria</t>
-  </si>
-  <si>
     <t>It consists of detecting which subprocesses have a higher cycle time, or a higher average cycle time, ... etc; either calculating some type of measurements or making a graph.</t>
   </si>
   <si>
-    <t>Identify activities as bottlenecks applying temporal performance criteria and statistical measures</t>
-  </si>
-  <si>
     <t>It consists of detecting which activities have a higher processing time, or a higher average processing time, or increase the average processing time of the variants more ... etc; either by calculating some type of measures in addition to taking into account the frequency with which they occur.</t>
   </si>
   <si>
-    <t>Identify organizational units as bottlenecks applying temporal performance criteria</t>
-  </si>
-  <si>
     <t>It consists of detecting which organizational units have a greater cycle time, or a greater average cycle time, or increase the average cycle time of the variants more ... etc; either calculating some type of measurements or making a graph.</t>
-  </si>
-  <si>
-    <t>Identify sub-processes with incorrect orders with respect to the happy path as bottlenecks</t>
   </si>
   <si>
     <t>It consists of determining subprocesses that have incorrect activity orders with respect to the happy path</t>
@@ -1853,6 +1835,24 @@
   </si>
   <si>
     <t>Definition of variants</t>
+  </si>
+  <si>
+    <t>Find bottlenecks</t>
+  </si>
+  <si>
+    <t>Find activities as bottlenecks applying temporal performance criteria</t>
+  </si>
+  <si>
+    <t>Find sub-processes as bottlenecks applying temporal performance criteria</t>
+  </si>
+  <si>
+    <t>Find organizational units as bottlenecks applying temporal performance criteria</t>
+  </si>
+  <si>
+    <t>Find activities as bottlenecks applying temporal performance criteria and statistical measures</t>
+  </si>
+  <si>
+    <t>Find sub-processes with incorrect orders with respect to the happy path as bottlenecks</t>
   </si>
 </sst>
 </file>
@@ -2018,6 +2018,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2025,24 +2038,11 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2384,8 +2384,8 @@
   <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,27 +2395,27 @@
     <col min="3" max="3" width="49.5703125" style="14" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" style="31" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" style="25" customWidth="1"/>
     <col min="7" max="7" width="39.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="24" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -2426,8 +2426,8 @@
       <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>525</v>
+      <c r="B2" s="28" t="s">
+        <v>519</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>4</v>
@@ -2437,32 +2437,32 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="22" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="23"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
@@ -2471,15 +2471,15 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="23"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
@@ -2490,25 +2490,25 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="15"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -2522,17 +2522,17 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="22" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -2543,15 +2543,15 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="15" t="s">
         <v>18</v>
       </c>
@@ -2564,8 +2564,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
@@ -2574,32 +2574,32 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="15" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="15" t="s">
         <v>23</v>
       </c>
@@ -2608,32 +2608,32 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="15" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="15" t="s">
         <v>26</v>
       </c>
@@ -2642,32 +2642,32 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="15" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
@@ -2676,78 +2676,78 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="15" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="22" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="9"/>
       <c r="C19" s="15" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="18" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="22" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2761,10 +2761,10 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="22" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2777,11 +2777,11 @@
       <c r="C22" s="15"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="29" t="s">
-        <v>363</v>
+      <c r="F22" s="23" t="s">
+        <v>357</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2795,10 +2795,10 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="22" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2812,10 +2812,10 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="22" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2829,17 +2829,17 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="22" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="28" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -2850,30 +2850,30 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="15" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
@@ -2882,15 +2882,15 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="15" t="s">
         <v>50</v>
       </c>
@@ -2899,15 +2899,15 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="15" t="s">
         <v>52</v>
       </c>
@@ -2916,15 +2916,15 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="15" t="s">
         <v>54</v>
       </c>
@@ -2933,15 +2933,15 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="15" t="s">
         <v>56</v>
       </c>
@@ -2950,15 +2950,15 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="15" t="s">
         <v>58</v>
       </c>
@@ -2967,15 +2967,15 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="15" t="s">
         <v>60</v>
       </c>
@@ -2984,15 +2984,15 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="15" t="s">
         <v>62</v>
       </c>
@@ -3001,15 +3001,15 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
       <c r="C36" s="15" t="s">
         <v>64</v>
       </c>
@@ -3018,15 +3018,15 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="15" t="s">
         <v>66</v>
       </c>
@@ -3035,15 +3035,15 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="15" t="s">
         <v>68</v>
       </c>
@@ -3054,31 +3054,31 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="28" t="s">
         <v>71</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="15" t="s">
         <v>72</v>
       </c>
@@ -3086,32 +3086,32 @@
         <v>73</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="15" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="15" t="s">
         <v>75</v>
       </c>
@@ -3122,17 +3122,17 @@
         <v>77</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="30" t="s">
         <v>79</v>
       </c>
       <c r="C43" s="15" t="s">
@@ -3143,15 +3143,15 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A44" s="23"/>
-      <c r="B44" s="27"/>
+      <c r="A44" s="28"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="15" t="s">
         <v>82</v>
       </c>
@@ -3162,15 +3162,15 @@
         <v>84</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="27"/>
+      <c r="A45" s="28"/>
+      <c r="B45" s="30"/>
       <c r="C45" s="15" t="s">
         <v>85</v>
       </c>
@@ -3181,8 +3181,8 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
-      <c r="B46" s="27"/>
+      <c r="A46" s="28"/>
+      <c r="B46" s="30"/>
       <c r="C46" s="15" t="s">
         <v>87</v>
       </c>
@@ -3191,15 +3191,15 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
-      <c r="B47" s="27"/>
+      <c r="A47" s="28"/>
+      <c r="B47" s="30"/>
       <c r="C47" s="15" t="s">
         <v>89</v>
       </c>
@@ -3208,15 +3208,15 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-      <c r="B48" s="27"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="30"/>
       <c r="C48" s="15" t="s">
         <v>91</v>
       </c>
@@ -3225,15 +3225,15 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="27"/>
+      <c r="A49" s="28"/>
+      <c r="B49" s="30"/>
       <c r="C49" s="15" t="s">
         <v>93</v>
       </c>
@@ -3244,10 +3244,10 @@
         <v>95</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3261,17 +3261,17 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="22" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
+      <c r="A51" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="23" t="s">
+      <c r="B51" s="28" t="s">
         <v>99</v>
       </c>
       <c r="C51" s="15" t="s">
@@ -3284,15 +3284,15 @@
         <v>102</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="23"/>
-      <c r="B52" s="23"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="15" t="s">
         <v>103</v>
       </c>
@@ -3303,15 +3303,15 @@
         <v>105</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
-      <c r="B53" s="23"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="15" t="s">
         <v>106</v>
       </c>
@@ -3320,15 +3320,15 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
-      <c r="B54" s="23"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="15" t="s">
         <v>108</v>
       </c>
@@ -3339,15 +3339,15 @@
         <v>110</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
-      <c r="B55" s="23"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="15" t="s">
         <v>111</v>
       </c>
@@ -3358,15 +3358,15 @@
         <v>113</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-      <c r="B56" s="23"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="15" t="s">
         <v>114</v>
       </c>
@@ -3377,15 +3377,15 @@
         <v>116</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-      <c r="B57" s="23"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="15" t="s">
         <v>117</v>
       </c>
@@ -3396,17 +3396,17 @@
         <v>119</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B58" s="23" t="s">
+      <c r="B58" s="28" t="s">
         <v>121</v>
       </c>
       <c r="C58" s="15" t="s">
@@ -3417,32 +3417,32 @@
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
-      <c r="B59" s="23"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="15" t="s">
         <v>124</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
-      <c r="B60" s="23"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="15" t="s">
         <v>126</v>
       </c>
@@ -3451,27 +3451,27 @@
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
-      <c r="B61" s="23"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="15" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3479,16 +3479,16 @@
         <v>128</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -3502,10 +3502,10 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="22" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3519,10 +3519,10 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3536,10 +3536,10 @@
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="22" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -3555,10 +3555,10 @@
         <v>137</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3572,10 +3572,10 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3589,27 +3589,27 @@
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="22" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="22" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3623,10 +3623,10 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="22" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3640,10 +3640,10 @@
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="22" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="G71" s="16" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3657,17 +3657,17 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="22" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A73" s="23" t="s">
+      <c r="A73" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="28" t="s">
         <v>150</v>
       </c>
       <c r="C73" s="15" t="s">
@@ -3678,15 +3678,15 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
-      <c r="B74" s="23"/>
+      <c r="A74" s="28"/>
+      <c r="B74" s="28"/>
       <c r="C74" s="15" t="s">
         <v>153</v>
       </c>
@@ -3695,32 +3695,32 @@
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="G74" s="16" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="23"/>
-      <c r="B75" s="23"/>
+      <c r="A75" s="28"/>
+      <c r="B75" s="28"/>
       <c r="C75" s="15" t="s">
         <v>155</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="23"/>
-      <c r="B76" s="23"/>
+      <c r="A76" s="28"/>
+      <c r="B76" s="28"/>
       <c r="C76" s="15" t="s">
         <v>156</v>
       </c>
@@ -3731,48 +3731,48 @@
         <v>158</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A77" s="23" t="s">
-        <v>308</v>
-      </c>
-      <c r="B77" s="24" t="s">
-        <v>309</v>
+      <c r="A77" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="B77" s="29" t="s">
+        <v>303</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="23"/>
-      <c r="B78" s="24"/>
+      <c r="A78" s="28"/>
+      <c r="B78" s="29"/>
       <c r="C78" s="15" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="G78" s="17" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3786,17 +3786,17 @@
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="23" t="s">
+      <c r="A80" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="B80" s="23" t="s">
+      <c r="B80" s="28" t="s">
         <v>162</v>
       </c>
       <c r="C80" s="15" t="s">
@@ -3807,15 +3807,15 @@
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
+      <c r="A81" s="28"/>
+      <c r="B81" s="28"/>
       <c r="C81" s="15" t="s">
         <v>165</v>
       </c>
@@ -3823,18 +3823,18 @@
         <v>166</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A82" s="23"/>
-      <c r="B82" s="23"/>
+      <c r="A82" s="28"/>
+      <c r="B82" s="28"/>
       <c r="C82" s="15" t="s">
         <v>167</v>
       </c>
@@ -3843,34 +3843,34 @@
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A83" s="23"/>
-      <c r="B83" s="23"/>
+      <c r="A83" s="28"/>
+      <c r="B83" s="28"/>
       <c r="C83" s="15" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="23" t="s">
+      <c r="A84" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="B84" s="23" t="s">
+      <c r="B84" s="28" t="s">
         <v>170</v>
       </c>
       <c r="C84" s="15" t="s">
@@ -3881,45 +3881,45 @@
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="A85" s="23"/>
-      <c r="B85" s="23"/>
-      <c r="C85" s="23" t="s">
+      <c r="A85" s="28"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="D85" s="24" t="s">
+      <c r="D85" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="E85" s="24"/>
+      <c r="E85" s="29"/>
       <c r="F85" s="1" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A86" s="23"/>
-      <c r="B86" s="23"/>
-      <c r="C86" s="23"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
+      <c r="A86" s="28"/>
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
       <c r="F86" s="1" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A87" s="23"/>
-      <c r="B87" s="23"/>
+      <c r="A87" s="28"/>
+      <c r="B87" s="28"/>
       <c r="C87" s="15" t="s">
         <v>175</v>
       </c>
@@ -3928,15 +3928,15 @@
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="23"/>
-      <c r="B88" s="23"/>
+      <c r="A88" s="28"/>
+      <c r="B88" s="28"/>
       <c r="C88" s="15" t="s">
         <v>177</v>
       </c>
@@ -3947,8 +3947,8 @@
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="23"/>
-      <c r="B89" s="23"/>
+      <c r="A89" s="28"/>
+      <c r="B89" s="28"/>
       <c r="C89" s="15" t="s">
         <v>179</v>
       </c>
@@ -3959,8 +3959,8 @@
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="23"/>
-      <c r="B90" s="23"/>
+      <c r="A90" s="28"/>
+      <c r="B90" s="28"/>
       <c r="C90" s="15" t="s">
         <v>181</v>
       </c>
@@ -3971,92 +3971,92 @@
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="23"/>
-      <c r="B91" s="23"/>
+      <c r="A91" s="28"/>
+      <c r="B91" s="28"/>
       <c r="C91" s="15" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A92" s="23" t="s">
+      <c r="A92" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="B92" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="B92" s="23" t="s">
+      <c r="C92" s="15" t="s">
+        <v>525</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="23"/>
-      <c r="B93" s="23"/>
+      <c r="A93" s="28"/>
+      <c r="B93" s="28"/>
       <c r="C93" s="15" t="s">
-        <v>187</v>
+        <v>526</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
-      <c r="B94" s="23"/>
+      <c r="A94" s="28"/>
+      <c r="B94" s="28"/>
       <c r="C94" s="15" t="s">
-        <v>189</v>
+        <v>528</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A95" s="23"/>
-      <c r="B95" s="23"/>
+      <c r="A95" s="28"/>
+      <c r="B95" s="28"/>
       <c r="C95" s="15" t="s">
-        <v>191</v>
+        <v>527</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="23"/>
-      <c r="B96" s="23"/>
+      <c r="A96" s="28"/>
+      <c r="B96" s="28"/>
       <c r="C96" s="15" t="s">
-        <v>193</v>
+        <v>529</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
     <row r="97" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C97" s="15"/>
       <c r="D97" s="1"/>
@@ -4065,10 +4065,10 @@
     </row>
     <row r="98" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C98" s="15"/>
       <c r="D98" s="1"/>
@@ -4076,98 +4076,98 @@
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A99" s="23" t="s">
+      <c r="A99" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="B99" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="C99" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A100" s="28"/>
+      <c r="B100" s="28"/>
+      <c r="C100" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D100" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="B99" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A100" s="23"/>
-      <c r="B100" s="23"/>
-      <c r="C100" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A101" s="23"/>
-      <c r="B101" s="23"/>
+      <c r="A101" s="28"/>
+      <c r="B101" s="28"/>
       <c r="C101" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A102" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="B102" s="28"/>
+      <c r="C102" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E102" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="F102" s="1"/>
+    </row>
+    <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A103" s="28"/>
+      <c r="B103" s="28"/>
+      <c r="C103" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="D103" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A102" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="B102" s="23"/>
-      <c r="C102" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E102" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F102" s="1"/>
-    </row>
-    <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="23"/>
-      <c r="B103" s="23"/>
-      <c r="C103" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C104" s="15"/>
       <c r="D104" s="1"/>
@@ -4175,136 +4175,136 @@
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:7" s="6" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="23" t="s">
-        <v>297</v>
-      </c>
-      <c r="B105" s="23" t="s">
-        <v>298</v>
+      <c r="A105" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="B105" s="28" t="s">
+        <v>292</v>
       </c>
       <c r="C105" s="15" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F105" s="22"/>
       <c r="G105" s="16"/>
     </row>
     <row r="106" spans="1:7" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="23"/>
-      <c r="B106" s="23"/>
+      <c r="A106" s="28"/>
+      <c r="B106" s="28"/>
       <c r="C106" s="15" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="22"/>
       <c r="G106" s="16"/>
     </row>
     <row r="107" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="23"/>
-      <c r="B107" s="23"/>
+      <c r="A107" s="28"/>
+      <c r="B107" s="28"/>
       <c r="C107" s="15" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="F107" s="22"/>
       <c r="G107" s="16"/>
     </row>
     <row r="108" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="23"/>
-      <c r="B108" s="23"/>
+      <c r="A108" s="28"/>
+      <c r="B108" s="28"/>
       <c r="C108" s="15" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="F108" s="22"/>
       <c r="G108" s="16"/>
     </row>
     <row r="109" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C109" s="15"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F109" s="22" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="25" t="s">
-        <v>305</v>
-      </c>
-      <c r="B110" s="23" t="s">
-        <v>306</v>
+      <c r="A110" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="B110" s="28" t="s">
+        <v>300</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="25"/>
-      <c r="B111" s="23"/>
+      <c r="A111" s="31"/>
+      <c r="B111" s="28"/>
       <c r="C111" s="15" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="25"/>
-      <c r="B112" s="23"/>
+      <c r="A112" s="31"/>
+      <c r="B112" s="28"/>
       <c r="C112" s="15" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="F112" s="1"/>
     </row>
     <row r="113" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C113" s="15"/>
       <c r="D113" s="1"/>
@@ -4318,29 +4318,29 @@
     </row>
     <row r="114" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C114" s="15"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F114" s="1" t="s">
         <v>146</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C115" s="15"/>
       <c r="D115" s="1"/>
@@ -4348,165 +4348,165 @@
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="B116" s="23" t="s">
-        <v>233</v>
+      <c r="A116" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B116" s="28" t="s">
+        <v>227</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="23"/>
-      <c r="B117" s="23"/>
+      <c r="A117" s="28"/>
+      <c r="B117" s="28"/>
       <c r="C117" s="15" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="G117" s="16" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="23"/>
-      <c r="B118" s="23"/>
+      <c r="A118" s="28"/>
+      <c r="B118" s="28"/>
       <c r="C118" s="15" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A119" s="23"/>
-      <c r="B119" s="23"/>
+      <c r="A119" s="28"/>
+      <c r="B119" s="28"/>
       <c r="C119" s="15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="G119" s="16" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="23"/>
-      <c r="B120" s="23"/>
+      <c r="A120" s="28"/>
+      <c r="B120" s="28"/>
       <c r="C120" s="15" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="23"/>
-      <c r="B121" s="23"/>
+      <c r="A121" s="28"/>
+      <c r="B121" s="28"/>
       <c r="C121" s="15" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C122" s="15"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="F122" s="22" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="G122" s="16" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="23" t="s">
-        <v>245</v>
-      </c>
-      <c r="B123" s="23" t="s">
-        <v>246</v>
+      <c r="A123" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="B123" s="28" t="s">
+        <v>240</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="23"/>
-      <c r="B124" s="23"/>
+      <c r="A124" s="28"/>
+      <c r="B124" s="28"/>
       <c r="C124" s="15" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="G124" s="16" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="23"/>
-      <c r="B125" s="23"/>
+      <c r="A125" s="28"/>
+      <c r="B125" s="28"/>
       <c r="C125" s="15" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C126" s="15"/>
       <c r="D126" s="1"/>
@@ -4515,10 +4515,10 @@
     </row>
     <row r="127" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="C127" s="15"/>
       <c r="D127" s="1"/>
@@ -4527,85 +4527,85 @@
     </row>
     <row r="128" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C128" s="15"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="F128" s="22" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="G128" s="16" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="C129" s="15"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F129" s="22" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="23" t="s">
-        <v>259</v>
-      </c>
-      <c r="B130" s="23" t="s">
-        <v>260</v>
+      <c r="A130" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="B130" s="28" t="s">
+        <v>254</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="G130" s="16" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="23"/>
-      <c r="B131" s="23"/>
+      <c r="A131" s="28"/>
+      <c r="B131" s="28"/>
       <c r="C131" s="15" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="G131" s="16" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="23"/>
-      <c r="B132" s="23"/>
+      <c r="A132" s="28"/>
+      <c r="B132" s="28"/>
       <c r="C132" s="15" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -4613,154 +4613,165 @@
     </row>
     <row r="133" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="C133" s="15"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="22" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="G133" s="16" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="23" t="s">
-        <v>276</v>
-      </c>
-      <c r="B134" s="23" t="s">
-        <v>277</v>
+      <c r="A134" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B134" s="28" t="s">
+        <v>271</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
     </row>
     <row r="135" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="23"/>
-      <c r="B135" s="23"/>
+      <c r="A135" s="28"/>
+      <c r="B135" s="28"/>
       <c r="C135" s="15" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="23"/>
-      <c r="B136" s="23"/>
+      <c r="A136" s="28"/>
+      <c r="B136" s="28"/>
       <c r="C136" s="15" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="F136" s="1"/>
     </row>
     <row r="137" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="23"/>
-      <c r="B137" s="23"/>
+      <c r="A137" s="28"/>
+      <c r="B137" s="28"/>
       <c r="C137" s="15" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="F137" s="1"/>
     </row>
     <row r="138" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="25" t="s">
-        <v>270</v>
-      </c>
-      <c r="B138" s="23" t="s">
-        <v>271</v>
+      <c r="A138" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="B138" s="28" t="s">
+        <v>265</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="25"/>
-      <c r="B139" s="23"/>
+      <c r="A139" s="31"/>
+      <c r="B139" s="28"/>
       <c r="C139" s="15" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="G139" s="15" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="25"/>
-      <c r="B140" s="23"/>
+      <c r="A140" s="31"/>
+      <c r="B140" s="28"/>
       <c r="C140" s="15" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="G140" s="22" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A8:A19"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="B138:B140"/>
+    <mergeCell ref="A130:A132"/>
+    <mergeCell ref="B130:B132"/>
+    <mergeCell ref="A116:A121"/>
+    <mergeCell ref="B116:B121"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="B134:B137"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A123:A125"/>
+    <mergeCell ref="B123:B125"/>
     <mergeCell ref="B84:B91"/>
     <mergeCell ref="A84:A91"/>
     <mergeCell ref="B2:B5"/>
@@ -4773,28 +4784,17 @@
     <mergeCell ref="B51:B57"/>
     <mergeCell ref="A73:A76"/>
     <mergeCell ref="B73:B76"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="B134:B137"/>
-    <mergeCell ref="A92:A96"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A123:A125"/>
-    <mergeCell ref="B123:B125"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="B138:B140"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="B130:B132"/>
-    <mergeCell ref="A116:A121"/>
-    <mergeCell ref="B116:B121"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A8:A19"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A80:A83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4802,21 +4802,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -5000,31 +4985,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5280F00-08C5-4424-8C69-5F59D5F29D10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5040,4 +5016,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated operationg coding and table of annotations
The name of some operations have been changed in order to understand them easier.
</commit_message>
<xml_diff>
--- a/OperationCoding.xlsx
+++ b/OperationCoding.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Trabajo\BPI Challenge\bpi-challenge-performance-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9712D6-B1B6-4130-96D7-A993C683A353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F96E45D-EC7C-49FC-9869-FF8DD2A61F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-630" yWindow="255" windowWidth="22800" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -727,9 +727,6 @@
     <t>Log con nuevos atributos o subconjunto de eventos</t>
   </si>
   <si>
-    <t>Represent scatterplot</t>
-  </si>
-  <si>
     <t>It consists of representing a measure in one axis (for example, resource) and in the other axis a different mesaure (for example, activity).</t>
   </si>
   <si>
@@ -839,9 +836,6 @@
     <t>Get process map from the previous question</t>
   </si>
   <si>
-    <t>Represent heatmaps</t>
-  </si>
-  <si>
     <t>It consists of showing figures that relate the intensity with which two characteristics occur (for example, Cycle Time and activities) indicating by colors the intensity with which two specific values of these characteristics occur.</t>
   </si>
   <si>
@@ -861,9 +855,6 @@
   </si>
   <si>
     <t>It consists of locating the units that require a greater or lesser cycle time</t>
-  </si>
-  <si>
-    <t>Represent linear tendency of cycle time</t>
   </si>
   <si>
     <t>it consists in plotting a two axis graph where one of them is cycle time</t>
@@ -1853,6 +1844,15 @@
   </si>
   <si>
     <t>Find sub-processes with incorrect orders with respect to the happy path as bottlenecks</t>
+  </si>
+  <si>
+    <t>Represent linear tendency of cycle time with respect an attribute</t>
+  </si>
+  <si>
+    <t>Represent scatterplot of cycle time and an attribute</t>
+  </si>
+  <si>
+    <t>Represent heat maps of cycle time and an attribute</t>
   </si>
 </sst>
 </file>
@@ -1950,7 +1950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2025,10 +2025,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2038,10 +2035,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2384,8 +2387,8 @@
   <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,16 +2404,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>520</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>522</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>523</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>0</v>
@@ -2423,11 +2426,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>519</v>
+      <c r="B2" s="27" t="s">
+        <v>516</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>4</v>
@@ -2437,32 +2440,32 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="27"/>
       <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="22" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
@@ -2471,15 +2474,15 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
@@ -2490,25 +2493,25 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="15"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -2522,17 +2525,17 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="22" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -2543,15 +2546,15 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="15" t="s">
         <v>18</v>
       </c>
@@ -2564,8 +2567,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
@@ -2574,32 +2577,32 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="15" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="15" t="s">
         <v>23</v>
       </c>
@@ -2608,32 +2611,32 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="15" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="15" t="s">
         <v>26</v>
       </c>
@@ -2642,32 +2645,32 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="15" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
@@ -2676,78 +2679,78 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="15" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="22" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="9"/>
       <c r="C19" s="15" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="18" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="22" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2761,10 +2764,10 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="22" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2778,10 +2781,10 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="23" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2795,10 +2798,10 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="22" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2812,10 +2815,10 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="22" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2829,17 +2832,17 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="22" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -2850,30 +2853,30 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="15" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
@@ -2882,15 +2885,15 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="15" t="s">
         <v>50</v>
       </c>
@@ -2899,15 +2902,15 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
       <c r="C30" s="15" t="s">
         <v>52</v>
       </c>
@@ -2916,15 +2919,15 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="15" t="s">
         <v>54</v>
       </c>
@@ -2933,15 +2936,15 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="15" t="s">
         <v>56</v>
       </c>
@@ -2950,15 +2953,15 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="15" t="s">
         <v>58</v>
       </c>
@@ -2967,15 +2970,15 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="15" t="s">
         <v>60</v>
       </c>
@@ -2984,15 +2987,15 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="15" t="s">
         <v>62</v>
       </c>
@@ -3001,15 +3004,15 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>432</v>
-      </c>
     </row>
     <row r="36" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="15" t="s">
         <v>64</v>
       </c>
@@ -3018,15 +3021,15 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>432</v>
-      </c>
     </row>
     <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="15" t="s">
         <v>66</v>
       </c>
@@ -3035,15 +3038,15 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="15" t="s">
         <v>68</v>
       </c>
@@ -3054,31 +3057,31 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
+      <c r="A39" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="15" t="s">
         <v>72</v>
       </c>
@@ -3086,32 +3089,32 @@
         <v>73</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="15" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="15" t="s">
         <v>75</v>
       </c>
@@ -3122,14 +3125,14 @@
         <v>77</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="27" t="s">
         <v>78</v>
       </c>
       <c r="B43" s="30" t="s">
@@ -3143,14 +3146,14 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
+      <c r="A44" s="27"/>
       <c r="B44" s="30"/>
       <c r="C44" s="15" t="s">
         <v>82</v>
@@ -3162,14 +3165,14 @@
         <v>84</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
+      <c r="A45" s="27"/>
       <c r="B45" s="30"/>
       <c r="C45" s="15" t="s">
         <v>85</v>
@@ -3181,7 +3184,7 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="30"/>
       <c r="C46" s="15" t="s">
         <v>87</v>
@@ -3191,14 +3194,14 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
+      <c r="A47" s="27"/>
       <c r="B47" s="30"/>
       <c r="C47" s="15" t="s">
         <v>89</v>
@@ -3208,14 +3211,14 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
+      <c r="A48" s="27"/>
       <c r="B48" s="30"/>
       <c r="C48" s="15" t="s">
         <v>91</v>
@@ -3225,14 +3228,14 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
+      <c r="A49" s="27"/>
       <c r="B49" s="30"/>
       <c r="C49" s="15" t="s">
         <v>93</v>
@@ -3244,10 +3247,10 @@
         <v>95</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3261,17 +3264,17 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="22" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="27" t="s">
         <v>99</v>
       </c>
       <c r="C51" s="15" t="s">
@@ -3284,15 +3287,15 @@
         <v>102</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
-      <c r="B52" s="28"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
       <c r="C52" s="15" t="s">
         <v>103</v>
       </c>
@@ -3303,15 +3306,15 @@
         <v>105</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="15" t="s">
         <v>106</v>
       </c>
@@ -3320,15 +3323,15 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="28"/>
-      <c r="B54" s="28"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
       <c r="C54" s="15" t="s">
         <v>108</v>
       </c>
@@ -3339,15 +3342,15 @@
         <v>110</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>365</v>
-      </c>
     </row>
     <row r="55" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
-      <c r="B55" s="28"/>
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
       <c r="C55" s="15" t="s">
         <v>111</v>
       </c>
@@ -3358,15 +3361,15 @@
         <v>113</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
-      <c r="B56" s="28"/>
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="15" t="s">
         <v>114</v>
       </c>
@@ -3377,15 +3380,15 @@
         <v>116</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
-      <c r="B57" s="28"/>
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="15" t="s">
         <v>117</v>
       </c>
@@ -3396,17 +3399,17 @@
         <v>119</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
+      <c r="A58" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="27" t="s">
         <v>121</v>
       </c>
       <c r="C58" s="15" t="s">
@@ -3417,32 +3420,32 @@
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="28"/>
-      <c r="B59" s="28"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
       <c r="C59" s="15" t="s">
         <v>124</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
-      <c r="B60" s="28"/>
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
       <c r="C60" s="15" t="s">
         <v>126</v>
       </c>
@@ -3451,27 +3454,27 @@
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="28"/>
-      <c r="B61" s="28"/>
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
       <c r="C61" s="15" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3479,16 +3482,16 @@
         <v>128</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -3502,10 +3505,10 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="22" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3519,10 +3522,10 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3536,10 +3539,10 @@
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="22" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -3555,10 +3558,10 @@
         <v>137</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3572,10 +3575,10 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3589,27 +3592,27 @@
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="22" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="22" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3623,10 +3626,10 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="22" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3640,10 +3643,10 @@
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="22" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G71" s="16" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3657,17 +3660,17 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="22" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
+      <c r="A73" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="B73" s="27" t="s">
         <v>150</v>
       </c>
       <c r="C73" s="15" t="s">
@@ -3678,15 +3681,15 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="28"/>
-      <c r="B74" s="28"/>
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
       <c r="C74" s="15" t="s">
         <v>153</v>
       </c>
@@ -3695,32 +3698,32 @@
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="G74" s="16" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="28"/>
-      <c r="B75" s="28"/>
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
       <c r="C75" s="15" t="s">
         <v>155</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="28"/>
-      <c r="B76" s="28"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
       <c r="C76" s="15" t="s">
         <v>156</v>
       </c>
@@ -3731,48 +3734,48 @@
         <v>158</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A77" s="28" t="s">
+      <c r="A77" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="C77" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="B77" s="29" t="s">
-        <v>303</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>305</v>
-      </c>
       <c r="D77" s="5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="28"/>
-      <c r="B78" s="29"/>
+      <c r="A78" s="27"/>
+      <c r="B78" s="28"/>
       <c r="C78" s="15" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="G78" s="17" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3786,17 +3789,17 @@
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="28" t="s">
+      <c r="A80" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="B80" s="28" t="s">
+      <c r="B80" s="27" t="s">
         <v>162</v>
       </c>
       <c r="C80" s="15" t="s">
@@ -3807,15 +3810,15 @@
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A81" s="28"/>
-      <c r="B81" s="28"/>
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
       <c r="C81" s="15" t="s">
         <v>165</v>
       </c>
@@ -3823,18 +3826,18 @@
         <v>166</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A82" s="28"/>
-      <c r="B82" s="28"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="15" t="s">
         <v>167</v>
       </c>
@@ -3843,34 +3846,34 @@
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A83" s="28"/>
-      <c r="B83" s="28"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
       <c r="C83" s="15" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
+      <c r="A84" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="B84" s="28" t="s">
+      <c r="B84" s="27" t="s">
         <v>170</v>
       </c>
       <c r="C84" s="15" t="s">
@@ -3881,45 +3884,45 @@
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="A85" s="28"/>
-      <c r="B85" s="28"/>
-      <c r="C85" s="28" t="s">
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="D85" s="29" t="s">
+      <c r="D85" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="E85" s="29"/>
+      <c r="E85" s="28"/>
       <c r="F85" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A86" s="28"/>
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="29"/>
-      <c r="E86" s="29"/>
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="28"/>
       <c r="F86" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A87" s="28"/>
-      <c r="B87" s="28"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
       <c r="C87" s="15" t="s">
         <v>175</v>
       </c>
@@ -3928,15 +3931,15 @@
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="28"/>
-      <c r="B88" s="28"/>
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
       <c r="C88" s="15" t="s">
         <v>177</v>
       </c>
@@ -3947,8 +3950,8 @@
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="28"/>
-      <c r="B89" s="28"/>
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
       <c r="C89" s="15" t="s">
         <v>179</v>
       </c>
@@ -3959,8 +3962,8 @@
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
-      <c r="B90" s="28"/>
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
       <c r="C90" s="15" t="s">
         <v>181</v>
       </c>
@@ -3971,43 +3974,43 @@
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="28"/>
-      <c r="B91" s="28"/>
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
       <c r="C91" s="15" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
-        <v>524</v>
-      </c>
-      <c r="B92" s="28" t="s">
+      <c r="A92" s="27" t="s">
+        <v>521</v>
+      </c>
+      <c r="B92" s="27" t="s">
         <v>183</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>184</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="28"/>
-      <c r="B93" s="28"/>
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
       <c r="C93" s="15" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>185</v>
@@ -4016,10 +4019,10 @@
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A94" s="28"/>
-      <c r="B94" s="28"/>
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
       <c r="C94" s="15" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>186</v>
@@ -4028,10 +4031,10 @@
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A95" s="28"/>
-      <c r="B95" s="28"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
       <c r="C95" s="15" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>187</v>
@@ -4040,10 +4043,10 @@
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="28"/>
-      <c r="B96" s="28"/>
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
       <c r="C96" s="15" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>188</v>
@@ -4053,10 +4056,10 @@
     </row>
     <row r="97" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C97" s="15"/>
       <c r="D97" s="1"/>
@@ -4076,10 +4079,10 @@
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A99" s="28" t="s">
+      <c r="A99" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="B99" s="28" t="s">
+      <c r="B99" s="27" t="s">
         <v>192</v>
       </c>
       <c r="C99" s="15" t="s">
@@ -4092,15 +4095,15 @@
         <v>195</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A100" s="28"/>
-      <c r="B100" s="28"/>
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
       <c r="C100" s="15" t="s">
         <v>196</v>
       </c>
@@ -4109,15 +4112,15 @@
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A101" s="28"/>
-      <c r="B101" s="28"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
       <c r="C101" s="15" t="s">
         <v>198</v>
       </c>
@@ -4128,17 +4131,17 @@
         <v>200</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A102" s="28" t="s">
+      <c r="A102" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="B102" s="28"/>
+      <c r="B102" s="27"/>
       <c r="C102" s="21" t="s">
         <v>202</v>
       </c>
@@ -4151,8 +4154,8 @@
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="28"/>
-      <c r="B103" s="28"/>
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
       <c r="C103" s="21" t="s">
         <v>205</v>
       </c>
@@ -4164,10 +4167,10 @@
     </row>
     <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C104" s="15"/>
       <c r="D104" s="1"/>
@@ -4175,11 +4178,11 @@
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:7" s="6" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="28" t="s">
-        <v>291</v>
-      </c>
-      <c r="B105" s="28" t="s">
-        <v>292</v>
+      <c r="A105" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="B105" s="27" t="s">
+        <v>289</v>
       </c>
       <c r="C105" s="15" t="s">
         <v>207</v>
@@ -4194,44 +4197,44 @@
       <c r="G105" s="16"/>
     </row>
     <row r="106" spans="1:7" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="28"/>
-      <c r="B106" s="28"/>
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
       <c r="C106" s="15" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="22"/>
       <c r="G106" s="16"/>
     </row>
     <row r="107" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="28"/>
-      <c r="B107" s="28"/>
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
       <c r="C107" s="15" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F107" s="22"/>
       <c r="G107" s="16"/>
     </row>
     <row r="108" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="28"/>
-      <c r="B108" s="28"/>
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
       <c r="C108" s="15" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F108" s="22"/>
       <c r="G108" s="16"/>
@@ -4256,11 +4259,11 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="31" t="s">
-        <v>299</v>
-      </c>
-      <c r="B110" s="28" t="s">
-        <v>300</v>
+      <c r="A110" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="B110" s="27" t="s">
+        <v>297</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>215</v>
@@ -4274,28 +4277,28 @@
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="31"/>
-      <c r="B111" s="28"/>
+      <c r="A111" s="29"/>
+      <c r="B111" s="27"/>
       <c r="C111" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D111" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>301</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="31"/>
-      <c r="B112" s="28"/>
+      <c r="A112" s="29"/>
+      <c r="B112" s="27"/>
       <c r="C112" s="15" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F112" s="1"/>
     </row>
@@ -4336,11 +4339,11 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="15" t="s">
+      <c r="A115" s="26" t="s">
+        <v>528</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>225</v>
       </c>
       <c r="C115" s="15"/>
       <c r="D115" s="1"/>
@@ -4348,165 +4351,165 @@
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="28" t="s">
+      <c r="A116" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B116" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="B116" s="28" t="s">
+      <c r="C116" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="C116" s="15" t="s">
-        <v>228</v>
-      </c>
       <c r="D116" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="28"/>
-      <c r="B117" s="28"/>
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
       <c r="C117" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G117" s="16" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="28"/>
-      <c r="B118" s="28"/>
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
       <c r="C118" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A119" s="28"/>
-      <c r="B119" s="28"/>
+      <c r="A119" s="27"/>
+      <c r="B119" s="27"/>
       <c r="C119" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="F119" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G119" s="16" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="28"/>
-      <c r="B120" s="28"/>
+      <c r="A120" s="27"/>
+      <c r="B120" s="27"/>
       <c r="C120" s="15" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="28"/>
-      <c r="B121" s="28"/>
+      <c r="A121" s="27"/>
+      <c r="B121" s="27"/>
       <c r="C121" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="C122" s="15"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="F122" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="G122" s="16" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="F122" s="22" t="s">
-        <v>396</v>
-      </c>
-      <c r="G122" s="16" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="28" t="s">
+      <c r="B123" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="B123" s="28" t="s">
+      <c r="C123" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C123" s="15" t="s">
+      <c r="D123" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="28"/>
-      <c r="B124" s="28"/>
+      <c r="A124" s="27"/>
+      <c r="B124" s="27"/>
       <c r="C124" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D124" s="1" t="s">
+      <c r="F124" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G124" s="16" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A125" s="27"/>
+      <c r="B125" s="27"/>
+      <c r="C125" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="F124" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G124" s="16" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="28"/>
-      <c r="B125" s="28"/>
-      <c r="C125" s="15" t="s">
+      <c r="D125" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C126" s="15"/>
       <c r="D126" s="1"/>
@@ -4515,10 +4518,10 @@
     </row>
     <row r="127" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C127" s="15"/>
       <c r="D127" s="1"/>
@@ -4527,229 +4530,258 @@
     </row>
     <row r="128" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="C128" s="15"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F128" s="22" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G128" s="16" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="B129" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>251</v>
       </c>
       <c r="C129" s="15"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F129" s="22" t="s">
+        <v>391</v>
+      </c>
+      <c r="G129" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="F129" s="22" t="s">
-        <v>394</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="28" t="s">
+      <c r="B130" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="B130" s="28" t="s">
+      <c r="C130" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C130" s="15" t="s">
+      <c r="D130" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G130" s="16" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="28"/>
-      <c r="B131" s="28"/>
+      <c r="A131" s="27"/>
+      <c r="B131" s="27"/>
       <c r="C131" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="D131" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G131" s="16" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="28"/>
-      <c r="B132" s="28"/>
+      <c r="A132" s="27"/>
+      <c r="B132" s="27"/>
       <c r="C132" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
     <row r="133" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A133" s="15" t="s">
-        <v>260</v>
+      <c r="A133" s="26" t="s">
+        <v>529</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C133" s="15"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="22" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G133" s="16" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="28" t="s">
+      <c r="A134" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B134" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="C134" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="D134" s="11" t="s">
         <v>270</v>
-      </c>
-      <c r="B134" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="C134" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="D134" s="11" t="s">
-        <v>273</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
     </row>
     <row r="135" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="28"/>
-      <c r="B135" s="28"/>
+      <c r="A135" s="27"/>
+      <c r="B135" s="27"/>
       <c r="C135" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="28"/>
-      <c r="B136" s="28"/>
+      <c r="A136" s="27"/>
+      <c r="B136" s="27"/>
       <c r="C136" s="15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F136" s="1"/>
     </row>
     <row r="137" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="28"/>
-      <c r="B137" s="28"/>
+      <c r="A137" s="27"/>
+      <c r="B137" s="27"/>
       <c r="C137" s="15" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F137" s="1"/>
     </row>
     <row r="138" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="31" t="s">
-        <v>264</v>
-      </c>
-      <c r="B138" s="28" t="s">
-        <v>265</v>
+      <c r="A138" s="29" t="s">
+        <v>262</v>
+      </c>
+      <c r="B138" s="27" t="s">
+        <v>263</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="31"/>
-      <c r="B139" s="28"/>
+      <c r="A139" s="29"/>
+      <c r="B139" s="27"/>
       <c r="C139" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G139" s="15" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="31"/>
-      <c r="B140" s="28"/>
+      <c r="A140" s="29"/>
+      <c r="B140" s="27"/>
       <c r="C140" s="15" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F140" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G140" s="22" t="s">
         <v>412</v>
-      </c>
-      <c r="G140" s="22" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
-        <v>268</v>
+        <v>527</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A8:A19"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="B84:B91"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A26:A38"/>
+    <mergeCell ref="B26:B38"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B49"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="B51:B57"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A123:A125"/>
+    <mergeCell ref="B123:B125"/>
+    <mergeCell ref="A102:A103"/>
     <mergeCell ref="C85:C86"/>
     <mergeCell ref="D85:D86"/>
     <mergeCell ref="E85:E86"/>
@@ -4766,35 +4798,6 @@
     <mergeCell ref="A134:A137"/>
     <mergeCell ref="B134:B137"/>
     <mergeCell ref="A92:A96"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A123:A125"/>
-    <mergeCell ref="B123:B125"/>
-    <mergeCell ref="B84:B91"/>
-    <mergeCell ref="A84:A91"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A26:A38"/>
-    <mergeCell ref="B26:B38"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B43:B49"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="B51:B57"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A8:A19"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A80:A83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4802,6 +4805,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -4985,22 +5003,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5280F00-08C5-4424-8C69-5F59D5F29D10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5016,28 +5043,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/isa-group/bpi-challenge-performance-analysis"
This reverts commit c0e457b91cd276fdc5e57219426dc7e14c549908, reversing
changes made to b98e1ebd552e7982d8984270151c1573fbdbdbf1.
</commit_message>
<xml_diff>
--- a/OperationCoding.xlsx
+++ b/OperationCoding.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Trabajo\BPI Challenge\bpi-challenge-performance-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F96E45D-EC7C-49FC-9869-FF8DD2A61F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9712D6-B1B6-4130-96D7-A993C683A353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-630" yWindow="255" windowWidth="22800" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -727,6 +727,9 @@
     <t>Log con nuevos atributos o subconjunto de eventos</t>
   </si>
   <si>
+    <t>Represent scatterplot</t>
+  </si>
+  <si>
     <t>It consists of representing a measure in one axis (for example, resource) and in the other axis a different mesaure (for example, activity).</t>
   </si>
   <si>
@@ -836,6 +839,9 @@
     <t>Get process map from the previous question</t>
   </si>
   <si>
+    <t>Represent heatmaps</t>
+  </si>
+  <si>
     <t>It consists of showing figures that relate the intensity with which two characteristics occur (for example, Cycle Time and activities) indicating by colors the intensity with which two specific values of these characteristics occur.</t>
   </si>
   <si>
@@ -855,6 +861,9 @@
   </si>
   <si>
     <t>It consists of locating the units that require a greater or lesser cycle time</t>
+  </si>
+  <si>
+    <t>Represent linear tendency of cycle time</t>
   </si>
   <si>
     <t>it consists in plotting a two axis graph where one of them is cycle time</t>
@@ -1844,15 +1853,6 @@
   </si>
   <si>
     <t>Find sub-processes with incorrect orders with respect to the happy path as bottlenecks</t>
-  </si>
-  <si>
-    <t>Represent linear tendency of cycle time with respect an attribute</t>
-  </si>
-  <si>
-    <t>Represent scatterplot of cycle time and an attribute</t>
-  </si>
-  <si>
-    <t>Represent heat maps of cycle time and an attribute</t>
   </si>
 </sst>
 </file>
@@ -1950,7 +1950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2025,7 +2025,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2035,16 +2038,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2387,8 +2384,8 @@
   <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,16 +2401,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>0</v>
@@ -2426,11 +2423,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>516</v>
+      <c r="B2" s="28" t="s">
+        <v>519</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>4</v>
@@ -2440,32 +2437,32 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="22" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
@@ -2474,15 +2471,15 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="27"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
       <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
@@ -2493,25 +2490,25 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="15"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -2525,17 +2522,17 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="22" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="28" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -2546,15 +2543,15 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="15" t="s">
         <v>18</v>
       </c>
@@ -2567,8 +2564,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
@@ -2577,32 +2574,32 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="15" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="15" t="s">
         <v>23</v>
       </c>
@@ -2611,32 +2608,32 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="15" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="15" t="s">
         <v>26</v>
       </c>
@@ -2645,32 +2642,32 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="15" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
+      <c r="A16" s="28"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
@@ -2679,78 +2676,78 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="15" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="22" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="9"/>
       <c r="C19" s="15" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="18" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="22" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2764,10 +2761,10 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="22" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2781,10 +2778,10 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="23" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2798,10 +2795,10 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="22" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2815,10 +2812,10 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="22" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2832,17 +2829,17 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="22" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="28" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -2853,30 +2850,30 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="15" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
@@ -2885,15 +2882,15 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="15" t="s">
         <v>50</v>
       </c>
@@ -2902,15 +2899,15 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="27"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="15" t="s">
         <v>52</v>
       </c>
@@ -2919,15 +2916,15 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="27"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="15" t="s">
         <v>54</v>
       </c>
@@ -2936,15 +2933,15 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="27"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="15" t="s">
         <v>56</v>
       </c>
@@ -2953,15 +2950,15 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="15" t="s">
         <v>58</v>
       </c>
@@ -2970,15 +2967,15 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="15" t="s">
         <v>60</v>
       </c>
@@ -2987,15 +2984,15 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="27"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="15" t="s">
         <v>62</v>
       </c>
@@ -3004,15 +3001,15 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
-      <c r="B36" s="27"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="28"/>
       <c r="C36" s="15" t="s">
         <v>64</v>
       </c>
@@ -3021,15 +3018,15 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
-      <c r="B37" s="27"/>
+      <c r="A37" s="28"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="15" t="s">
         <v>66</v>
       </c>
@@ -3038,15 +3035,15 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="15" t="s">
         <v>68</v>
       </c>
@@ -3057,31 +3054,31 @@
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
+      <c r="A39" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="28" t="s">
         <v>71</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="15" t="s">
         <v>72</v>
       </c>
@@ -3089,32 +3086,32 @@
         <v>73</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
+      <c r="A41" s="28"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="15" t="s">
         <v>74</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="15" t="s">
         <v>75</v>
       </c>
@@ -3125,14 +3122,14 @@
         <v>77</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="28" t="s">
         <v>78</v>
       </c>
       <c r="B43" s="30" t="s">
@@ -3146,14 +3143,14 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
+      <c r="A44" s="28"/>
       <c r="B44" s="30"/>
       <c r="C44" s="15" t="s">
         <v>82</v>
@@ -3165,14 +3162,14 @@
         <v>84</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
+      <c r="A45" s="28"/>
       <c r="B45" s="30"/>
       <c r="C45" s="15" t="s">
         <v>85</v>
@@ -3184,7 +3181,7 @@
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
+      <c r="A46" s="28"/>
       <c r="B46" s="30"/>
       <c r="C46" s="15" t="s">
         <v>87</v>
@@ -3194,14 +3191,14 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
+      <c r="A47" s="28"/>
       <c r="B47" s="30"/>
       <c r="C47" s="15" t="s">
         <v>89</v>
@@ -3211,14 +3208,14 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
+      <c r="A48" s="28"/>
       <c r="B48" s="30"/>
       <c r="C48" s="15" t="s">
         <v>91</v>
@@ -3228,14 +3225,14 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="27"/>
+      <c r="A49" s="28"/>
       <c r="B49" s="30"/>
       <c r="C49" s="15" t="s">
         <v>93</v>
@@ -3247,10 +3244,10 @@
         <v>95</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3264,17 +3261,17 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="22" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+      <c r="A51" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="28" t="s">
         <v>99</v>
       </c>
       <c r="C51" s="15" t="s">
@@ -3287,15 +3284,15 @@
         <v>102</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
-      <c r="B52" s="27"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="15" t="s">
         <v>103</v>
       </c>
@@ -3306,15 +3303,15 @@
         <v>105</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="15" t="s">
         <v>106</v>
       </c>
@@ -3323,15 +3320,15 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
-      <c r="B54" s="27"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="15" t="s">
         <v>108</v>
       </c>
@@ -3342,15 +3339,15 @@
         <v>110</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="15" t="s">
         <v>111</v>
       </c>
@@ -3361,15 +3358,15 @@
         <v>113</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="27"/>
-      <c r="B56" s="27"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="15" t="s">
         <v>114</v>
       </c>
@@ -3380,15 +3377,15 @@
         <v>116</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="15" t="s">
         <v>117</v>
       </c>
@@ -3399,17 +3396,17 @@
         <v>119</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="27" t="s">
+      <c r="A58" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="28" t="s">
         <v>121</v>
       </c>
       <c r="C58" s="15" t="s">
@@ -3420,32 +3417,32 @@
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="15" t="s">
         <v>124</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
-      <c r="B60" s="27"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="15" t="s">
         <v>126</v>
       </c>
@@ -3454,27 +3451,27 @@
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="27"/>
-      <c r="B61" s="27"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="15" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3482,16 +3479,16 @@
         <v>128</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -3505,10 +3502,10 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="22" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3522,10 +3519,10 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3539,10 +3536,10 @@
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="22" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -3558,10 +3555,10 @@
         <v>137</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3575,10 +3572,10 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3592,27 +3589,27 @@
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="22" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="22" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3626,10 +3623,10 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="22" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3643,10 +3640,10 @@
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="22" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G71" s="16" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3660,17 +3657,17 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="22" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A73" s="27" t="s">
+      <c r="A73" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B73" s="27" t="s">
+      <c r="B73" s="28" t="s">
         <v>150</v>
       </c>
       <c r="C73" s="15" t="s">
@@ -3681,15 +3678,15 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="27"/>
-      <c r="B74" s="27"/>
+      <c r="A74" s="28"/>
+      <c r="B74" s="28"/>
       <c r="C74" s="15" t="s">
         <v>153</v>
       </c>
@@ -3698,32 +3695,32 @@
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="G74" s="16" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="27"/>
-      <c r="B75" s="27"/>
+      <c r="A75" s="28"/>
+      <c r="B75" s="28"/>
       <c r="C75" s="15" t="s">
         <v>155</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="27"/>
-      <c r="B76" s="27"/>
+      <c r="A76" s="28"/>
+      <c r="B76" s="28"/>
       <c r="C76" s="15" t="s">
         <v>156</v>
       </c>
@@ -3734,48 +3731,48 @@
         <v>158</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A77" s="27" t="s">
-        <v>299</v>
-      </c>
-      <c r="B77" s="28" t="s">
-        <v>300</v>
+      <c r="A77" s="28" t="s">
+        <v>302</v>
+      </c>
+      <c r="B77" s="29" t="s">
+        <v>303</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="27"/>
-      <c r="B78" s="28"/>
+      <c r="A78" s="28"/>
+      <c r="B78" s="29"/>
       <c r="C78" s="15" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="G78" s="17" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3789,17 +3786,17 @@
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="27" t="s">
+      <c r="A80" s="28" t="s">
         <v>161</v>
       </c>
-      <c r="B80" s="27" t="s">
+      <c r="B80" s="28" t="s">
         <v>162</v>
       </c>
       <c r="C80" s="15" t="s">
@@ -3810,15 +3807,15 @@
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A81" s="27"/>
-      <c r="B81" s="27"/>
+      <c r="A81" s="28"/>
+      <c r="B81" s="28"/>
       <c r="C81" s="15" t="s">
         <v>165</v>
       </c>
@@ -3826,18 +3823,18 @@
         <v>166</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A82" s="27"/>
-      <c r="B82" s="27"/>
+      <c r="A82" s="28"/>
+      <c r="B82" s="28"/>
       <c r="C82" s="15" t="s">
         <v>167</v>
       </c>
@@ -3846,34 +3843,34 @@
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A83" s="27"/>
-      <c r="B83" s="27"/>
+      <c r="A83" s="28"/>
+      <c r="B83" s="28"/>
       <c r="C83" s="15" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G83" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="G83" s="1" t="s">
-        <v>509</v>
-      </c>
     </row>
     <row r="84" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="27" t="s">
+      <c r="A84" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="B84" s="27" t="s">
+      <c r="B84" s="28" t="s">
         <v>170</v>
       </c>
       <c r="C84" s="15" t="s">
@@ -3884,45 +3881,45 @@
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="A85" s="27"/>
-      <c r="B85" s="27"/>
-      <c r="C85" s="27" t="s">
+      <c r="A85" s="28"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="D85" s="28" t="s">
+      <c r="D85" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="E85" s="28"/>
+      <c r="E85" s="29"/>
       <c r="F85" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A86" s="27"/>
-      <c r="B86" s="27"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="28"/>
+      <c r="A86" s="28"/>
+      <c r="B86" s="28"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
       <c r="F86" s="1" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A87" s="27"/>
-      <c r="B87" s="27"/>
+      <c r="A87" s="28"/>
+      <c r="B87" s="28"/>
       <c r="C87" s="15" t="s">
         <v>175</v>
       </c>
@@ -3931,15 +3928,15 @@
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="27"/>
-      <c r="B88" s="27"/>
+      <c r="A88" s="28"/>
+      <c r="B88" s="28"/>
       <c r="C88" s="15" t="s">
         <v>177</v>
       </c>
@@ -3950,8 +3947,8 @@
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="27"/>
-      <c r="B89" s="27"/>
+      <c r="A89" s="28"/>
+      <c r="B89" s="28"/>
       <c r="C89" s="15" t="s">
         <v>179</v>
       </c>
@@ -3962,8 +3959,8 @@
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="27"/>
-      <c r="B90" s="27"/>
+      <c r="A90" s="28"/>
+      <c r="B90" s="28"/>
       <c r="C90" s="15" t="s">
         <v>181</v>
       </c>
@@ -3974,43 +3971,43 @@
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="27"/>
-      <c r="B91" s="27"/>
+      <c r="A91" s="28"/>
+      <c r="B91" s="28"/>
       <c r="C91" s="15" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A92" s="27" t="s">
-        <v>521</v>
-      </c>
-      <c r="B92" s="27" t="s">
+      <c r="A92" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="B92" s="28" t="s">
         <v>183</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>184</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="27"/>
-      <c r="B93" s="27"/>
+      <c r="A93" s="28"/>
+      <c r="B93" s="28"/>
       <c r="C93" s="15" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>185</v>
@@ -4019,10 +4016,10 @@
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A94" s="27"/>
-      <c r="B94" s="27"/>
+      <c r="A94" s="28"/>
+      <c r="B94" s="28"/>
       <c r="C94" s="15" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>186</v>
@@ -4031,10 +4028,10 @@
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A95" s="27"/>
-      <c r="B95" s="27"/>
+      <c r="A95" s="28"/>
+      <c r="B95" s="28"/>
       <c r="C95" s="15" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>187</v>
@@ -4043,10 +4040,10 @@
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="27"/>
-      <c r="B96" s="27"/>
+      <c r="A96" s="28"/>
+      <c r="B96" s="28"/>
       <c r="C96" s="15" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>188</v>
@@ -4056,10 +4053,10 @@
     </row>
     <row r="97" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C97" s="15"/>
       <c r="D97" s="1"/>
@@ -4079,10 +4076,10 @@
       <c r="F98" s="1"/>
     </row>
     <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A99" s="27" t="s">
+      <c r="A99" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="B99" s="27" t="s">
+      <c r="B99" s="28" t="s">
         <v>192</v>
       </c>
       <c r="C99" s="15" t="s">
@@ -4095,15 +4092,15 @@
         <v>195</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A100" s="27"/>
-      <c r="B100" s="27"/>
+      <c r="A100" s="28"/>
+      <c r="B100" s="28"/>
       <c r="C100" s="15" t="s">
         <v>196</v>
       </c>
@@ -4112,15 +4109,15 @@
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A101" s="27"/>
-      <c r="B101" s="27"/>
+      <c r="A101" s="28"/>
+      <c r="B101" s="28"/>
       <c r="C101" s="15" t="s">
         <v>198</v>
       </c>
@@ -4131,17 +4128,17 @@
         <v>200</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A102" s="27" t="s">
+      <c r="A102" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="B102" s="27"/>
+      <c r="B102" s="28"/>
       <c r="C102" s="21" t="s">
         <v>202</v>
       </c>
@@ -4154,8 +4151,8 @@
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="27"/>
-      <c r="B103" s="27"/>
+      <c r="A103" s="28"/>
+      <c r="B103" s="28"/>
       <c r="C103" s="21" t="s">
         <v>205</v>
       </c>
@@ -4167,10 +4164,10 @@
     </row>
     <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C104" s="15"/>
       <c r="D104" s="1"/>
@@ -4178,11 +4175,11 @@
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:7" s="6" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="B105" s="27" t="s">
-        <v>289</v>
+      <c r="A105" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="B105" s="28" t="s">
+        <v>292</v>
       </c>
       <c r="C105" s="15" t="s">
         <v>207</v>
@@ -4197,44 +4194,44 @@
       <c r="G105" s="16"/>
     </row>
     <row r="106" spans="1:7" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="27"/>
-      <c r="B106" s="27"/>
+      <c r="A106" s="28"/>
+      <c r="B106" s="28"/>
       <c r="C106" s="15" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="22"/>
       <c r="G106" s="16"/>
     </row>
     <row r="107" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="27"/>
-      <c r="B107" s="27"/>
+      <c r="A107" s="28"/>
+      <c r="B107" s="28"/>
       <c r="C107" s="15" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="F107" s="22"/>
       <c r="G107" s="16"/>
     </row>
     <row r="108" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="27"/>
-      <c r="B108" s="27"/>
+      <c r="A108" s="28"/>
+      <c r="B108" s="28"/>
       <c r="C108" s="15" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F108" s="22"/>
       <c r="G108" s="16"/>
@@ -4259,11 +4256,11 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="29" t="s">
-        <v>296</v>
-      </c>
-      <c r="B110" s="27" t="s">
-        <v>297</v>
+      <c r="A110" s="31" t="s">
+        <v>299</v>
+      </c>
+      <c r="B110" s="28" t="s">
+        <v>300</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>215</v>
@@ -4277,28 +4274,28 @@
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="29"/>
-      <c r="B111" s="27"/>
+      <c r="A111" s="31"/>
+      <c r="B111" s="28"/>
       <c r="C111" s="15" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="29"/>
-      <c r="B112" s="27"/>
+      <c r="A112" s="31"/>
+      <c r="B112" s="28"/>
       <c r="C112" s="15" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="F112" s="1"/>
     </row>
@@ -4339,11 +4336,11 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="26" t="s">
-        <v>528</v>
+      <c r="A115" s="15" t="s">
+        <v>224</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C115" s="15"/>
       <c r="D115" s="1"/>
@@ -4351,165 +4348,165 @@
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="27" t="s">
-        <v>225</v>
-      </c>
-      <c r="B116" s="27" t="s">
+      <c r="A116" s="28" t="s">
         <v>226</v>
       </c>
+      <c r="B116" s="28" t="s">
+        <v>227</v>
+      </c>
       <c r="C116" s="15" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
     </row>
     <row r="117" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="27"/>
-      <c r="B117" s="27"/>
+      <c r="A117" s="28"/>
+      <c r="B117" s="28"/>
       <c r="C117" s="15" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="G117" s="16" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="27"/>
-      <c r="B118" s="27"/>
+      <c r="A118" s="28"/>
+      <c r="B118" s="28"/>
       <c r="C118" s="15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
     </row>
     <row r="119" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A119" s="27"/>
-      <c r="B119" s="27"/>
+      <c r="A119" s="28"/>
+      <c r="B119" s="28"/>
       <c r="C119" s="15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="G119" s="16" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="27"/>
-      <c r="B120" s="27"/>
+      <c r="A120" s="28"/>
+      <c r="B120" s="28"/>
       <c r="C120" s="15" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="27"/>
-      <c r="B121" s="27"/>
+      <c r="A121" s="28"/>
+      <c r="B121" s="28"/>
       <c r="C121" s="15" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C122" s="15"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F122" s="22" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="G122" s="16" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="B123" s="27" t="s">
+      <c r="A123" s="28" t="s">
         <v>239</v>
       </c>
+      <c r="B123" s="28" t="s">
+        <v>240</v>
+      </c>
       <c r="C123" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="27"/>
-      <c r="B124" s="27"/>
+      <c r="A124" s="28"/>
+      <c r="B124" s="28"/>
       <c r="C124" s="15" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="G124" s="16" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="27"/>
-      <c r="B125" s="27"/>
+      <c r="A125" s="28"/>
+      <c r="B125" s="28"/>
       <c r="C125" s="15" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="C126" s="15"/>
       <c r="D126" s="1"/>
@@ -4518,10 +4515,10 @@
     </row>
     <row r="127" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="C127" s="15"/>
       <c r="D127" s="1"/>
@@ -4530,235 +4527,251 @@
     </row>
     <row r="128" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C128" s="15"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F128" s="22" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="G128" s="16" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C129" s="15"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F129" s="22" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="B130" s="27" t="s">
+      <c r="A130" s="28" t="s">
         <v>253</v>
       </c>
+      <c r="B130" s="28" t="s">
+        <v>254</v>
+      </c>
       <c r="C130" s="15" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="G130" s="16" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="27"/>
-      <c r="B131" s="27"/>
+      <c r="A131" s="28"/>
+      <c r="B131" s="28"/>
       <c r="C131" s="15" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="G131" s="16" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="27"/>
-      <c r="B132" s="27"/>
+      <c r="A132" s="28"/>
+      <c r="B132" s="28"/>
       <c r="C132" s="15" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
     <row r="133" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A133" s="26" t="s">
-        <v>529</v>
+      <c r="A133" s="15" t="s">
+        <v>260</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C133" s="15"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="22" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="G133" s="16" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="B134" s="27" t="s">
-        <v>268</v>
+      <c r="A134" s="28" t="s">
+        <v>270</v>
+      </c>
+      <c r="B134" s="28" t="s">
+        <v>271</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
     </row>
     <row r="135" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="27"/>
-      <c r="B135" s="27"/>
+      <c r="A135" s="28"/>
+      <c r="B135" s="28"/>
       <c r="C135" s="15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="27"/>
-      <c r="B136" s="27"/>
+      <c r="A136" s="28"/>
+      <c r="B136" s="28"/>
       <c r="C136" s="15" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="F136" s="1"/>
     </row>
     <row r="137" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="27"/>
-      <c r="B137" s="27"/>
+      <c r="A137" s="28"/>
+      <c r="B137" s="28"/>
       <c r="C137" s="15" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F137" s="1"/>
     </row>
     <row r="138" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="B138" s="27" t="s">
-        <v>263</v>
+      <c r="A138" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="B138" s="28" t="s">
+        <v>265</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="29"/>
-      <c r="B139" s="27"/>
+      <c r="A139" s="31"/>
+      <c r="B139" s="28"/>
       <c r="C139" s="15" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="G139" s="15" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="29"/>
-      <c r="B140" s="27"/>
+      <c r="A140" s="31"/>
+      <c r="B140" s="28"/>
       <c r="C140" s="15" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="G140" s="22" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="15" t="s">
-        <v>527</v>
+        <v>268</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A8:A19"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="B138:B140"/>
+    <mergeCell ref="A130:A132"/>
+    <mergeCell ref="B130:B132"/>
+    <mergeCell ref="A116:A121"/>
+    <mergeCell ref="B116:B121"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="A134:A137"/>
+    <mergeCell ref="B134:B137"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A123:A125"/>
+    <mergeCell ref="B123:B125"/>
     <mergeCell ref="B84:B91"/>
     <mergeCell ref="A84:A91"/>
     <mergeCell ref="B2:B5"/>
@@ -4775,29 +4788,13 @@
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="B58:B61"/>
     <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A123:A125"/>
-    <mergeCell ref="B123:B125"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A8:A19"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A49"/>
     <mergeCell ref="A102:A103"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="B138:B140"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="B130:B132"/>
-    <mergeCell ref="A116:A121"/>
-    <mergeCell ref="B116:B121"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="B134:B137"/>
-    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="A80:A83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4805,21 +4802,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -5003,31 +4985,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5280F00-08C5-4424-8C69-5F59D5F29D10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5043,4 +5016,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated operation coding and relocation of notebook
</commit_message>
<xml_diff>
--- a/OperationCoding.xlsx
+++ b/OperationCoding.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Trabajo\BPI Challenge\bpi-challenge-performance-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9712D6-B1B6-4130-96D7-A993C683A353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A73170-D5FB-4DD3-AC01-3CEE5A83D083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-630" yWindow="255" windowWidth="22800" windowHeight="9975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="531">
   <si>
     <t>Examples</t>
   </si>
@@ -727,9 +727,6 @@
     <t>Log con nuevos atributos o subconjunto de eventos</t>
   </si>
   <si>
-    <t>Represent scatterplot</t>
-  </si>
-  <si>
     <t>It consists of representing a measure in one axis (for example, resource) and in the other axis a different mesaure (for example, activity).</t>
   </si>
   <si>
@@ -808,9 +805,6 @@
 Representación de diagrama de cajas del cycle time calculado para cada log</t>
   </si>
   <si>
-    <t>Represent density of cycle time</t>
-  </si>
-  <si>
     <t>It consists of showing linearly the number of traces / events (Y-axis) that have a certain cycle time for sections (X axis)</t>
   </si>
   <si>
@@ -839,9 +833,6 @@
     <t>Get process map from the previous question</t>
   </si>
   <si>
-    <t>Represent heatmaps</t>
-  </si>
-  <si>
     <t>It consists of showing figures that relate the intensity with which two characteristics occur (for example, Cycle Time and activities) indicating by colors the intensity with which two specific values of these characteristics occur.</t>
   </si>
   <si>
@@ -861,9 +852,6 @@
   </si>
   <si>
     <t>It consists of locating the units that require a greater or lesser cycle time</t>
-  </si>
-  <si>
-    <t>Represent linear tendency of cycle time</t>
   </si>
   <si>
     <t>it consists in plotting a two axis graph where one of them is cycle time</t>
@@ -1853,6 +1841,21 @@
   </si>
   <si>
     <t>Find sub-processes with incorrect orders with respect to the happy path as bottlenecks</t>
+  </si>
+  <si>
+    <t>Represent heat maps of cycle time and an attribute</t>
+  </si>
+  <si>
+    <t>Represent linear tendency of cycle time with respect an attribute</t>
+  </si>
+  <si>
+    <t>Represent density diagram of cycle time</t>
+  </si>
+  <si>
+    <t>Represent scatterplot of cycle time and an attribute</t>
+  </si>
+  <si>
+    <t>It consists of grouping events depending on the values of attributes</t>
   </si>
 </sst>
 </file>
@@ -1950,7 +1953,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2025,11 +2028,11 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2038,10 +2041,16 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2384,8 +2393,8 @@
   <dimension ref="A1:G141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C97" sqref="C97"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,16 +2410,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>0</v>
@@ -2423,11 +2432,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="32" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>4</v>
@@ -2437,31 +2446,31 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="28"/>
       <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="22" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="28"/>
       <c r="C4" s="15" t="s">
         <v>7</v>
@@ -2471,14 +2480,14 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="28"/>
       <c r="C5" s="15" t="s">
         <v>9</v>
@@ -2490,25 +2499,29 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="15"/>
+        <v>341</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>530</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>341</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -2518,14 +2531,16 @@
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="26" t="s">
+        <v>12</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="22" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2543,10 +2558,10 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2574,27 +2589,27 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="28"/>
       <c r="B11" s="28"/>
       <c r="C11" s="15" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2608,27 +2623,27 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
       <c r="B13" s="28"/>
       <c r="C13" s="15" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2642,27 +2657,27 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="28"/>
       <c r="C15" s="15" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2676,10 +2691,10 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -2689,65 +2704,67 @@
         <v>31</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28"/>
       <c r="B18" s="28"/>
       <c r="C18" s="15" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="22" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="28"/>
       <c r="B19" s="9"/>
       <c r="C19" s="15" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="18" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="C20" s="15"/>
+        <v>308</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>307</v>
+      </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="22" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2757,14 +2774,16 @@
       <c r="B21" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="26" t="s">
+        <v>32</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="22" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2774,14 +2793,16 @@
       <c r="B22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="26" t="s">
+        <v>34</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="23" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2791,14 +2812,16 @@
       <c r="B23" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="26" t="s">
+        <v>36</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="22" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2808,14 +2831,16 @@
       <c r="B24" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="26" t="s">
+        <v>38</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="22" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2825,14 +2850,16 @@
       <c r="B25" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="22" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2850,10 +2877,10 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2865,10 +2892,10 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2882,10 +2909,10 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2899,10 +2926,10 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2916,10 +2943,10 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2933,10 +2960,10 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -2950,10 +2977,10 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -2967,10 +2994,10 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -2984,10 +3011,10 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3001,10 +3028,10 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3018,10 +3045,10 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3035,10 +3062,10 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3061,19 +3088,19 @@
         <v>71</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3086,10 +3113,10 @@
         <v>73</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3099,14 +3126,14 @@
         <v>74</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3122,17 +3149,17 @@
         <v>77</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="31" t="s">
         <v>79</v>
       </c>
       <c r="C43" s="15" t="s">
@@ -3143,15 +3170,15 @@
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
-      <c r="B44" s="30"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="15" t="s">
         <v>82</v>
       </c>
@@ -3162,15 +3189,15 @@
         <v>84</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
-      <c r="B45" s="30"/>
+      <c r="B45" s="31"/>
       <c r="C45" s="15" t="s">
         <v>85</v>
       </c>
@@ -3182,7 +3209,7 @@
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
-      <c r="B46" s="30"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="15" t="s">
         <v>87</v>
       </c>
@@ -3191,15 +3218,15 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="28"/>
-      <c r="B47" s="30"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="15" t="s">
         <v>89</v>
       </c>
@@ -3208,15 +3235,15 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="28"/>
-      <c r="B48" s="30"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="15" t="s">
         <v>91</v>
       </c>
@@ -3225,15 +3252,15 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="28"/>
-      <c r="B49" s="30"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="15" t="s">
         <v>93</v>
       </c>
@@ -3244,10 +3271,10 @@
         <v>95</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3257,14 +3284,16 @@
       <c r="B50" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="15"/>
+      <c r="C50" s="26" t="s">
+        <v>96</v>
+      </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="22" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G50" s="16" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3284,10 +3313,10 @@
         <v>102</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G51" s="15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3303,10 +3332,10 @@
         <v>105</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G52" s="16" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3320,10 +3349,10 @@
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3339,10 +3368,10 @@
         <v>110</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3358,10 +3387,10 @@
         <v>113</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3377,10 +3406,10 @@
         <v>116</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="G56" s="16" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3396,10 +3425,10 @@
         <v>119</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -3417,10 +3446,10 @@
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G58" s="16" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3430,11 +3459,11 @@
         <v>124</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>125</v>
@@ -3451,27 +3480,27 @@
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G60" s="16" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
       <c r="B61" s="28"/>
       <c r="C61" s="15" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3479,16 +3508,18 @@
         <v>128</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="C62" s="15"/>
+        <v>474</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>128</v>
+      </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="G62" s="16" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -3498,14 +3529,16 @@
       <c r="B63" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C63" s="15"/>
+      <c r="C63" s="26" t="s">
+        <v>129</v>
+      </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="22" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="G63" s="16" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3515,14 +3548,16 @@
       <c r="B64" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C64" s="15"/>
+      <c r="C64" s="26" t="s">
+        <v>131</v>
+      </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3532,14 +3567,16 @@
       <c r="B65" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C65" s="15"/>
+      <c r="C65" s="26" t="s">
+        <v>133</v>
+      </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="22" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -3549,16 +3586,18 @@
       <c r="B66" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="15"/>
+      <c r="C66" s="26" t="s">
+        <v>135</v>
+      </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1" t="s">
         <v>137</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="G66" s="16" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3568,14 +3607,16 @@
       <c r="B67" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C67" s="15"/>
+      <c r="C67" s="26" t="s">
+        <v>138</v>
+      </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="G67" s="16" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3585,31 +3626,35 @@
       <c r="B68" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C68" s="15"/>
+      <c r="C68" s="26" t="s">
+        <v>140</v>
+      </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="22" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G68" s="16" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C69" s="15"/>
+        <v>312</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>311</v>
+      </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="22" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="G69" s="16" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3619,14 +3664,16 @@
       <c r="B70" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C70" s="15"/>
+      <c r="C70" s="26" t="s">
+        <v>142</v>
+      </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="22" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3636,14 +3683,16 @@
       <c r="B71" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C71" s="15"/>
+      <c r="C71" s="26" t="s">
+        <v>144</v>
+      </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="22" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G71" s="16" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3653,14 +3702,16 @@
       <c r="B72" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="C72" s="15"/>
+      <c r="C72" s="26" t="s">
+        <v>147</v>
+      </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="22" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -3678,10 +3729,10 @@
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3695,10 +3746,10 @@
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G74" s="16" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3708,14 +3759,14 @@
         <v>155</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3731,48 +3782,48 @@
         <v>158</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G76" s="16" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B77" s="29" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="28"/>
       <c r="B78" s="29"/>
       <c r="C78" s="15" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G78" s="17" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3782,14 +3833,16 @@
       <c r="B79" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="15"/>
+      <c r="C79" s="26" t="s">
+        <v>159</v>
+      </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -3807,10 +3860,10 @@
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3823,13 +3876,13 @@
         <v>166</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3843,27 +3896,27 @@
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A83" s="28"/>
       <c r="B83" s="28"/>
       <c r="C83" s="15" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3881,10 +3934,10 @@
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="195" x14ac:dyDescent="0.25">
@@ -3898,10 +3951,10 @@
       </c>
       <c r="E85" s="29"/>
       <c r="F85" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -3911,10 +3964,10 @@
       <c r="D86" s="29"/>
       <c r="E86" s="29"/>
       <c r="F86" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -3928,10 +3981,10 @@
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3974,40 +4027,40 @@
       <c r="A91" s="28"/>
       <c r="B91" s="28"/>
       <c r="C91" s="15" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
     </row>
     <row r="92" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B92" s="28" t="s">
         <v>183</v>
       </c>
       <c r="C92" s="15" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>184</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A93" s="28"/>
       <c r="B93" s="28"/>
       <c r="C93" s="15" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>185</v>
@@ -4019,7 +4072,7 @@
       <c r="A94" s="28"/>
       <c r="B94" s="28"/>
       <c r="C94" s="15" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>186</v>
@@ -4031,7 +4084,7 @@
       <c r="A95" s="28"/>
       <c r="B95" s="28"/>
       <c r="C95" s="15" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>187</v>
@@ -4043,7 +4096,7 @@
       <c r="A96" s="28"/>
       <c r="B96" s="28"/>
       <c r="C96" s="15" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>188</v>
@@ -4053,12 +4106,14 @@
     </row>
     <row r="97" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>314</v>
-      </c>
-      <c r="C97" s="15"/>
+        <v>310</v>
+      </c>
+      <c r="C97" s="26" t="s">
+        <v>309</v>
+      </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
@@ -4070,7 +4125,9 @@
       <c r="B98" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C98" s="15"/>
+      <c r="C98" s="26" t="s">
+        <v>189</v>
+      </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
@@ -4092,10 +4149,10 @@
         <v>195</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -4109,10 +4166,10 @@
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -4128,10 +4185,10 @@
         <v>200</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -4164,22 +4221,24 @@
     </row>
     <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="C104" s="15"/>
+        <v>280</v>
+      </c>
+      <c r="C104" s="26" t="s">
+        <v>281</v>
+      </c>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
     </row>
     <row r="105" spans="1:7" s="6" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="28" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C105" s="15" t="s">
         <v>207</v>
@@ -4197,10 +4256,10 @@
       <c r="A106" s="28"/>
       <c r="B106" s="28"/>
       <c r="C106" s="15" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E106" s="4"/>
       <c r="F106" s="22"/>
@@ -4210,13 +4269,13 @@
       <c r="A107" s="28"/>
       <c r="B107" s="28"/>
       <c r="C107" s="15" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F107" s="22"/>
       <c r="G107" s="16"/>
@@ -4225,13 +4284,13 @@
       <c r="A108" s="28"/>
       <c r="B108" s="28"/>
       <c r="C108" s="15" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D108" s="10" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E108" s="10" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F108" s="22"/>
       <c r="G108" s="16"/>
@@ -4243,7 +4302,9 @@
       <c r="B109" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C109" s="15"/>
+      <c r="C109" s="26" t="s">
+        <v>210</v>
+      </c>
       <c r="D109" s="1"/>
       <c r="E109" s="1" t="s">
         <v>212</v>
@@ -4256,11 +4317,11 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="31" t="s">
-        <v>299</v>
+      <c r="A110" s="30" t="s">
+        <v>295</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>215</v>
@@ -4274,28 +4335,28 @@
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="31"/>
+      <c r="A111" s="30"/>
       <c r="B111" s="28"/>
       <c r="C111" s="15" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="31"/>
+      <c r="A112" s="30"/>
       <c r="B112" s="28"/>
       <c r="C112" s="15" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E112" s="10" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F112" s="1"/>
     </row>
@@ -4306,7 +4367,9 @@
       <c r="B113" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C113" s="15"/>
+      <c r="C113" s="26" t="s">
+        <v>218</v>
+      </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1" t="s">
@@ -4323,7 +4386,9 @@
       <c r="B114" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C114" s="15"/>
+      <c r="C114" s="26" t="s">
+        <v>220</v>
+      </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1" t="s">
         <v>222</v>
@@ -4336,29 +4401,31 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="15" t="s">
+      <c r="A115" s="26" t="s">
+        <v>529</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C115" s="15"/>
+      <c r="C115" s="26" t="s">
+        <v>529</v>
+      </c>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B116" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="B116" s="28" t="s">
+      <c r="C116" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="C116" s="15" t="s">
-        <v>228</v>
-      </c>
       <c r="D116" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
@@ -4367,27 +4434,27 @@
       <c r="A117" s="28"/>
       <c r="B117" s="28"/>
       <c r="C117" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="G117" s="16" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="28"/>
       <c r="B118" s="28"/>
       <c r="C118" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D118" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
@@ -4396,26 +4463,26 @@
       <c r="A119" s="28"/>
       <c r="B119" s="28"/>
       <c r="C119" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D119" s="1" t="s">
+      <c r="E119" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="F119" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="G119" s="16" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="28"/>
       <c r="B120" s="28"/>
       <c r="C120" s="15" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
@@ -4425,187 +4492,197 @@
       <c r="A121" s="28"/>
       <c r="B121" s="28"/>
       <c r="C121" s="15" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
     </row>
     <row r="122" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B122" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B122" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C122" s="15"/>
+      <c r="C122" s="26" t="s">
+        <v>235</v>
+      </c>
       <c r="D122" s="1"/>
       <c r="E122" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F122" s="22" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="G122" s="16" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="B123" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="B123" s="28" t="s">
+      <c r="C123" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C123" s="15" t="s">
+      <c r="D123" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A124" s="28"/>
       <c r="B124" s="28"/>
       <c r="C124" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D124" s="1" t="s">
-        <v>244</v>
-      </c>
       <c r="F124" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="G124" s="16" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A125" s="28"/>
       <c r="B125" s="28"/>
       <c r="C125" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="C126" s="15"/>
+        <v>333</v>
+      </c>
+      <c r="C126" s="26" t="s">
+        <v>332</v>
+      </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
     <row r="127" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="C127" s="15"/>
+        <v>340</v>
+      </c>
+      <c r="C127" s="26" t="s">
+        <v>342</v>
+      </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
     </row>
     <row r="128" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="B128" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B128" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="C128" s="15"/>
+      <c r="C128" s="26" t="s">
+        <v>246</v>
+      </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F128" s="22" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G128" s="16" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A129" s="15" t="s">
-        <v>250</v>
+        <v>528</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="C129" s="15"/>
+        <v>249</v>
+      </c>
+      <c r="C129" s="26" t="s">
+        <v>528</v>
+      </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F129" s="22" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="B130" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C130" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B130" s="28" t="s">
+      <c r="D130" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="C130" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G130" s="16" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A131" s="28"/>
       <c r="B131" s="28"/>
       <c r="C131" s="15" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="G131" s="16" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="28"/>
       <c r="B132" s="28"/>
       <c r="C132" s="15" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
@@ -4613,33 +4690,35 @@
     </row>
     <row r="133" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
-        <v>260</v>
+        <v>526</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C133" s="15"/>
+        <v>258</v>
+      </c>
+      <c r="C133" s="26" t="s">
+        <v>526</v>
+      </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="22" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="G133" s="16" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="28" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B134" s="28" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C134" s="20" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D134" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
@@ -4648,10 +4727,10 @@
       <c r="A135" s="28"/>
       <c r="B135" s="28"/>
       <c r="C135" s="15" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
@@ -4660,13 +4739,13 @@
       <c r="A136" s="28"/>
       <c r="B136" s="28"/>
       <c r="C136" s="15" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F136" s="1"/>
     </row>
@@ -4674,82 +4753,111 @@
       <c r="A137" s="28"/>
       <c r="B137" s="28"/>
       <c r="C137" s="15" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F137" s="1"/>
     </row>
     <row r="138" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="31" t="s">
-        <v>264</v>
+      <c r="A138" s="30" t="s">
+        <v>261</v>
       </c>
       <c r="B138" s="28" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E138" s="1"/>
       <c r="F138" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="G138" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="31"/>
+      <c r="A139" s="30"/>
       <c r="B139" s="28"/>
       <c r="C139" s="15" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G139" s="15" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="31"/>
+      <c r="A140" s="30"/>
       <c r="B140" s="28"/>
       <c r="C140" s="15" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="G140" s="22" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="15" t="s">
-        <v>268</v>
+      <c r="A141" s="26" t="s">
+        <v>527</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A8:A19"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A49"/>
+    <mergeCell ref="B84:B91"/>
+    <mergeCell ref="A84:A91"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A26:A38"/>
+    <mergeCell ref="B26:B38"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="B43:B49"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="B51:B57"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="B73:B76"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A123:A125"/>
+    <mergeCell ref="B123:B125"/>
+    <mergeCell ref="A102:A103"/>
     <mergeCell ref="C85:C86"/>
     <mergeCell ref="D85:D86"/>
     <mergeCell ref="E85:E86"/>
@@ -4766,35 +4874,6 @@
     <mergeCell ref="A134:A137"/>
     <mergeCell ref="B134:B137"/>
     <mergeCell ref="A92:A96"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A123:A125"/>
-    <mergeCell ref="B123:B125"/>
-    <mergeCell ref="B84:B91"/>
-    <mergeCell ref="A84:A91"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A26:A38"/>
-    <mergeCell ref="B26:B38"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B43:B49"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="B51:B57"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A8:A19"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A80:A83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4802,6 +4881,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -4985,15 +5073,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5001,6 +5080,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5280F00-08C5-4424-8C69-5F59D5F29D10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5014,14 +5101,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed question 1, 2 and 5 from BPI 2020
The operations of each case related with the question 1 and 2 have been merged since they both require the same process data. Some cases used information of question 1 to answer question 5, therefore in these cases some operations that they recycled of question 1 have also been added to question 5.
</commit_message>
<xml_diff>
--- a/OperationCoding.xlsx
+++ b/OperationCoding.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Trabajo\BPI Challenge\bpi-challenge-performance-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A73170-D5FB-4DD3-AC01-3CEE5A83D083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23752655-8A16-415B-AD8F-4EAF73CEBA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="528">
   <si>
     <t>Examples</t>
   </si>
@@ -237,12 +237,6 @@
   </si>
   <si>
     <t>It consists of calculating the cycle time of a part of the process for different groupings of traces</t>
-  </si>
-  <si>
-    <t>Get cycle time from the previous question</t>
-  </si>
-  <si>
-    <t>It consists of reusing some calculation of the cycle time made previously</t>
   </si>
   <si>
     <t>Calculate statistics</t>
@@ -828,9 +822,6 @@
   </si>
   <si>
     <t>It consists of generating a process map indicating the cycle time required by the activities.</t>
-  </si>
-  <si>
-    <t>Get process map from the previous question</t>
   </si>
   <si>
     <t>It consists of showing figures that relate the intensity with which two characteristics occur (for example, Cycle Time and activities) indicating by colors the intensity with which two specific values of these characteristics occur.</t>
@@ -1953,7 +1944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2035,22 +2026,25 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2390,11 +2384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2410,16 +2404,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>516</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>518</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>519</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>0</v>
@@ -2432,11 +2426,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>515</v>
+      <c r="B2" s="29" t="s">
+        <v>512</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>4</v>
@@ -2446,32 +2440,32 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="22" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
@@ -2480,15 +2474,15 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
@@ -2499,29 +2493,29 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -2537,17 +2531,17 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="22" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="29" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -2558,15 +2552,15 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="15" t="s">
         <v>18</v>
       </c>
@@ -2579,8 +2573,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
@@ -2589,32 +2583,32 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="15" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="15" t="s">
         <v>23</v>
       </c>
@@ -2623,32 +2617,32 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="15" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="15" t="s">
         <v>26</v>
       </c>
@@ -2657,32 +2651,32 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="15" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
@@ -2691,80 +2685,80 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="15" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="22" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G18" s="16" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="9"/>
       <c r="C19" s="15" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="18" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="22" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2780,10 +2774,10 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="22" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2799,10 +2793,10 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="23" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2818,10 +2812,10 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="22" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2837,10 +2831,10 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="22" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2856,17 +2850,17 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="22" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="29" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -2877,30 +2871,30 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="15" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
@@ -2909,15 +2903,15 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="15" t="s">
         <v>50</v>
       </c>
@@ -2926,15 +2920,15 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="15" t="s">
         <v>52</v>
       </c>
@@ -2943,15 +2937,15 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="15" t="s">
         <v>54</v>
       </c>
@@ -2960,15 +2954,15 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="15" t="s">
         <v>56</v>
       </c>
@@ -2977,15 +2971,15 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="15" t="s">
         <v>58</v>
       </c>
@@ -2994,15 +2988,15 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="28"/>
-      <c r="B34" s="28"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="15" t="s">
         <v>60</v>
       </c>
@@ -3011,15 +3005,15 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A35" s="28"/>
-      <c r="B35" s="28"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="15" t="s">
         <v>62</v>
       </c>
@@ -3028,176 +3022,176 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G35" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="G35" s="1" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="36" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="28"/>
-      <c r="B36" s="28"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="28" t="s">
         <v>65</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>428</v>
-      </c>
     </row>
     <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="28"/>
-      <c r="B37" s="28"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="28" t="s">
         <v>67</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>431</v>
-      </c>
       <c r="G39" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="28"/>
-      <c r="B40" s="28"/>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="15" t="s">
+      <c r="D41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="F41" s="1" t="s">
         <v>439</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="B42" s="28"/>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>77</v>
+      </c>
       <c r="C42" s="15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="31" t="s">
-        <v>79</v>
-      </c>
+    </row>
+    <row r="43" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A43" s="29"/>
+      <c r="B43" s="33"/>
       <c r="C43" s="15" t="s">
         <v>80</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="F43" s="1" t="s">
         <v>444</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A44" s="28"/>
-      <c r="B44" s="31"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="29"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="15" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="28"/>
-      <c r="B45" s="31"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="29"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="15" t="s">
         <v>85</v>
       </c>
@@ -3205,11 +3199,16 @@
         <v>86</v>
       </c>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="28"/>
-      <c r="B46" s="31"/>
+      <c r="F45" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="29"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="15" t="s">
         <v>87</v>
       </c>
@@ -3218,15 +3217,15 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>449</v>
-      </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
-      <c r="B47" s="31"/>
+      <c r="A47" s="29"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="15" t="s">
         <v>89</v>
       </c>
@@ -3235,294 +3234,296 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>451</v>
-      </c>
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
-      <c r="B48" s="31"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="33"/>
       <c r="C48" s="15" t="s">
         <v>91</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="F48" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="28"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D49" s="1" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="C49" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="G49" s="16" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C50" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="G50" s="16" t="s">
-        <v>472</v>
+      <c r="C50" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="G50" s="15" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" s="28" t="s">
-        <v>99</v>
-      </c>
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="15" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="G51" s="15" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
-      <c r="B52" s="28"/>
+        <v>103</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="G51" s="16" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E52" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="F52" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
-      <c r="B53" s="28"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
       <c r="C53" s="15" t="s">
         <v>106</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="F53" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="G53" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="28"/>
-      <c r="B54" s="28"/>
+    </row>
+    <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
       <c r="C54" s="15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>361</v>
+        <v>111</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="28"/>
-      <c r="B55" s="28"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
       <c r="C55" s="15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>404</v>
+        <v>451</v>
       </c>
       <c r="G55" s="16" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
-      <c r="B56" s="28"/>
+        <v>452</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="29"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="15" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F56" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="G56" s="16" t="s">
+      <c r="G57" s="16" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A57" s="28"/>
-      <c r="B57" s="28"/>
-      <c r="C57" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>121</v>
-      </c>
+    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="15" t="s">
         <v>122</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>123</v>
+        <v>276</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="G58" s="16" t="s">
-        <v>458</v>
+        <v>456</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="28"/>
-      <c r="B59" s="28"/>
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="15" t="s">
         <v>124</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>279</v>
+        <v>125</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="28"/>
-      <c r="B60" s="28"/>
+        <v>359</v>
+      </c>
+      <c r="G59" s="16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="29"/>
+      <c r="B60" s="29"/>
       <c r="C60" s="15" t="s">
-        <v>126</v>
+        <v>299</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>127</v>
+        <v>300</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="G60" s="16" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="28"/>
-      <c r="B61" s="28"/>
-      <c r="C61" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>447</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="C61" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>450</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>472</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>474</v>
-      </c>
       <c r="C62" s="26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="1" t="s">
+      <c r="F62" s="22" t="s">
+        <v>474</v>
+      </c>
+      <c r="G62" s="16" t="s">
         <v>475</v>
       </c>
-      <c r="G62" s="16" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>129</v>
       </c>
@@ -3534,14 +3535,14 @@
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="22" t="s">
+      <c r="F63" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G63" s="16" t="s">
         <v>477</v>
       </c>
-      <c r="G63" s="16" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
         <v>131</v>
       </c>
@@ -3553,51 +3554,51 @@
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="G64" s="16" t="s">
         <v>479</v>
       </c>
-      <c r="G64" s="16" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="16" t="s">
         <v>134</v>
       </c>
       <c r="C65" s="26" t="s">
         <v>133</v>
       </c>
       <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
+      <c r="E65" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="F65" s="22" t="s">
+        <v>480</v>
+      </c>
+      <c r="G65" s="16" t="s">
         <v>481</v>
       </c>
-      <c r="G65" s="16" t="s">
+    </row>
+    <row r="66" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B66" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="C66" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F66" s="22" t="s">
+      <c r="G66" s="16" t="s">
         <v>483</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3612,52 +3613,52 @@
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="1" t="s">
+      <c r="F67" s="22" t="s">
+        <v>484</v>
+      </c>
+      <c r="G67" s="16" t="s">
         <v>485</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
-        <v>140</v>
+        <v>308</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>141</v>
+        <v>309</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>140</v>
+        <v>308</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="G68" s="16" t="s">
         <v>487</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
-        <v>311</v>
+        <v>140</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>312</v>
+        <v>141</v>
       </c>
       <c r="C69" s="26" t="s">
-        <v>311</v>
+        <v>140</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="22" t="s">
+        <v>488</v>
+      </c>
+      <c r="G69" s="16" t="s">
         <v>489</v>
       </c>
-      <c r="G69" s="16" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
         <v>142</v>
       </c>
@@ -3670,79 +3671,77 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="22" t="s">
-        <v>491</v>
+        <v>355</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B71" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="B71" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="C71" s="26" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="22" t="s">
-        <v>358</v>
+        <v>491</v>
       </c>
       <c r="G71" s="16" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A72" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="C72" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="D72" s="1"/>
+      <c r="C72" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="E72" s="1"/>
-      <c r="F72" s="22" t="s">
-        <v>494</v>
+      <c r="F72" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A73" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="B73" s="28" t="s">
-        <v>150</v>
-      </c>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A73" s="29"/>
+      <c r="B73" s="29"/>
       <c r="C73" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="16" t="s">
         <v>152</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
-        <v>344</v>
+        <v>493</v>
       </c>
       <c r="G73" s="16" t="s">
-        <v>343</v>
+        <v>494</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="28"/>
-      <c r="B74" s="28"/>
+      <c r="A74" s="29"/>
+      <c r="B74" s="29"/>
       <c r="C74" s="15" t="s">
         <v>153</v>
       </c>
       <c r="D74" s="16" t="s">
-        <v>154</v>
+        <v>495</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
@@ -3753,226 +3752,226 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="28"/>
-      <c r="B75" s="28"/>
+      <c r="A75" s="29"/>
+      <c r="B75" s="29"/>
       <c r="C75" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D75" s="16" t="s">
-        <v>498</v>
-      </c>
-      <c r="E75" s="1"/>
+      <c r="E75" s="1" t="s">
+        <v>156</v>
+      </c>
       <c r="F75" s="1" t="s">
         <v>499</v>
       </c>
       <c r="G75" s="16" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A76" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="B76" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="G76" s="17" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="28"/>
-      <c r="B76" s="28"/>
-      <c r="C76" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="G76" s="16" t="s">
-        <v>501</v>
-      </c>
-    </row>
     <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A77" s="28" t="s">
-        <v>298</v>
-      </c>
-      <c r="B77" s="29" t="s">
-        <v>299</v>
-      </c>
+      <c r="A77" s="29"/>
+      <c r="B77" s="30"/>
       <c r="C77" s="15" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="28"/>
-      <c r="B78" s="29"/>
-      <c r="C78" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>306</v>
-      </c>
+      <c r="A78" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="G78" s="17" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A79" s="15" t="s">
+    <row r="79" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="D79" s="1"/>
+      <c r="C79" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>162</v>
+      </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="G79" s="17" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="B80" s="28" t="s">
-        <v>162</v>
-      </c>
+    </row>
+    <row r="80" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A80" s="29"/>
+      <c r="B80" s="29"/>
       <c r="C80" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D80" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E80" s="1"/>
+      <c r="E80" s="1" t="s">
+        <v>288</v>
+      </c>
       <c r="F80" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A81" s="28"/>
-      <c r="B81" s="28"/>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A81" s="29"/>
+      <c r="B81" s="29"/>
       <c r="C81" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="D81" s="4" t="s">
+      <c r="D81" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A82" s="28"/>
-      <c r="B82" s="28"/>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
       <c r="C82" s="15" t="s">
-        <v>167</v>
+        <v>289</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>168</v>
+        <v>290</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A83" s="28"/>
-      <c r="B83" s="28"/>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="29" t="s">
+        <v>168</v>
+      </c>
       <c r="C83" s="15" t="s">
-        <v>292</v>
+        <v>169</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>293</v>
+        <v>170</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
-        <v>169</v>
-      </c>
-      <c r="B84" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" s="15" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A84" s="29"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29" t="s">
         <v>171</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D84" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="E84" s="1"/>
+      <c r="E84" s="30"/>
       <c r="F84" s="1" t="s">
-        <v>513</v>
+        <v>353</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="A85" s="28"/>
-      <c r="B85" s="28"/>
-      <c r="C85" s="28" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A86" s="29"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="D85" s="29" t="s">
+      <c r="D86" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E85" s="29"/>
-      <c r="F85" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A86" s="28"/>
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="29"/>
-      <c r="E86" s="29"/>
+      <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A87" s="28"/>
-      <c r="B87" s="28"/>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
       <c r="C87" s="15" t="s">
         <v>175</v>
       </c>
@@ -3980,16 +3979,11 @@
         <v>176</v>
       </c>
       <c r="E87" s="1"/>
-      <c r="F87" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>365</v>
-      </c>
+      <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="28"/>
-      <c r="B88" s="28"/>
+      <c r="A88" s="29"/>
+      <c r="B88" s="29"/>
       <c r="C88" s="15" t="s">
         <v>177</v>
       </c>
@@ -4000,8 +3994,8 @@
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="28"/>
-      <c r="B89" s="28"/>
+      <c r="A89" s="29"/>
+      <c r="B89" s="29"/>
       <c r="C89" s="15" t="s">
         <v>179</v>
       </c>
@@ -4012,355 +4006,362 @@
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="28"/>
-      <c r="B90" s="28"/>
+      <c r="A90" s="29"/>
+      <c r="B90" s="29"/>
       <c r="C90" s="15" t="s">
-        <v>181</v>
+        <v>310</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>182</v>
+        <v>311</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="28"/>
-      <c r="B91" s="28"/>
+    <row r="91" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A91" s="29" t="s">
+        <v>517</v>
+      </c>
+      <c r="B91" s="29" t="s">
+        <v>181</v>
+      </c>
       <c r="C91" s="15" t="s">
-        <v>313</v>
+        <v>518</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>314</v>
+        <v>182</v>
       </c>
       <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-    </row>
-    <row r="92" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A92" s="28" t="s">
-        <v>520</v>
-      </c>
-      <c r="B92" s="28" t="s">
+      <c r="F91" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A92" s="29"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="15" t="s">
+        <v>519</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+    </row>
+    <row r="93" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A93" s="29"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="15" t="s">
         <v>521</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A93" s="28"/>
-      <c r="B93" s="28"/>
-      <c r="C93" s="15" t="s">
-        <v>522</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A94" s="28"/>
-      <c r="B94" s="28"/>
+    <row r="94" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A94" s="29"/>
+      <c r="B94" s="29"/>
       <c r="C94" s="15" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A95" s="28"/>
-      <c r="B95" s="28"/>
+    <row r="95" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A95" s="29"/>
+      <c r="B95" s="29"/>
       <c r="C95" s="15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="28"/>
-      <c r="B96" s="28"/>
-      <c r="C96" s="15" t="s">
-        <v>525</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>188</v>
-      </c>
+    <row r="96" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="C96" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>310</v>
+        <v>187</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>188</v>
       </c>
       <c r="C97" s="26" t="s">
-        <v>309</v>
+        <v>187</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A98" s="15" t="s">
+      <c r="A98" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="C98" s="26" t="s">
-        <v>189</v>
-      </c>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
+      <c r="C98" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A99" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="B99" s="28" t="s">
-        <v>192</v>
-      </c>
+      <c r="A99" s="29"/>
+      <c r="B99" s="29"/>
       <c r="C99" s="15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E99" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="G99" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A100" s="28"/>
-      <c r="B100" s="28"/>
+    </row>
+    <row r="100" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A100" s="29"/>
+      <c r="B100" s="29"/>
       <c r="C100" s="15" t="s">
         <v>196</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E100" s="1"/>
+      <c r="E100" s="1" t="s">
+        <v>198</v>
+      </c>
       <c r="F100" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G100" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="G100" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A101" s="28"/>
-      <c r="B101" s="28"/>
-      <c r="C101" s="15" t="s">
-        <v>198</v>
+    </row>
+    <row r="101" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A101" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="B101" s="29"/>
+      <c r="C101" s="21" t="s">
+        <v>200</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A102" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="B102" s="28"/>
+        <v>202</v>
+      </c>
+      <c r="F101" s="1"/>
+    </row>
+    <row r="102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="29"/>
+      <c r="B102" s="29"/>
       <c r="C102" s="21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E102" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="28"/>
-      <c r="B103" s="28"/>
-      <c r="C103" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>206</v>
-      </c>
+    <row r="103" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A103" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C103" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A104" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C104" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-    </row>
-    <row r="105" spans="1:7" s="6" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="28" t="s">
+    <row r="104" spans="1:7" s="6" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="B104" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F104" s="22"/>
+      <c r="G104" s="16"/>
+    </row>
+    <row r="105" spans="1:7" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="29"/>
+      <c r="B105" s="29"/>
+      <c r="C105" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="B105" s="28" t="s">
-        <v>288</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>207</v>
-      </c>
       <c r="D105" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="E105" s="4" t="s">
-        <v>209</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="E105" s="4"/>
       <c r="F105" s="22"/>
       <c r="G105" s="16"/>
     </row>
-    <row r="106" spans="1:7" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="28"/>
-      <c r="B106" s="28"/>
+    <row r="106" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="29"/>
+      <c r="B106" s="29"/>
       <c r="C106" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="E106" s="4"/>
+        <v>316</v>
+      </c>
+      <c r="D106" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="E106" s="10" t="s">
+        <v>317</v>
+      </c>
       <c r="F106" s="22"/>
       <c r="G106" s="16"/>
     </row>
     <row r="107" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="28"/>
-      <c r="B107" s="28"/>
+      <c r="A107" s="29"/>
+      <c r="B107" s="29"/>
       <c r="C107" s="15" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E107" s="10" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="F107" s="22"/>
       <c r="G107" s="16"/>
     </row>
-    <row r="108" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="28"/>
-      <c r="B108" s="28"/>
-      <c r="C108" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="D108" s="10" t="s">
+    <row r="108" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A108" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C108" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F108" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A109" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="B109" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F109" s="1"/>
+    </row>
+    <row r="110" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="34"/>
+      <c r="B110" s="29"/>
+      <c r="C110" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="D110" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+    </row>
+    <row r="111" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="34"/>
+      <c r="B111" s="29"/>
+      <c r="C111" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="E108" s="10" t="s">
+      <c r="D111" s="9" t="s">
         <v>327</v>
       </c>
-      <c r="F108" s="22"/>
-      <c r="G108" s="16"/>
-    </row>
-    <row r="109" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A109" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C109" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F109" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A110" s="30" t="s">
-        <v>295</v>
-      </c>
-      <c r="B110" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="D110" s="5" t="s">
+      <c r="E111" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="F111" s="1"/>
+    </row>
+    <row r="112" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A112" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="E110" s="1" t="s">
+      <c r="B112" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F110" s="1"/>
-    </row>
-    <row r="111" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="30"/>
-      <c r="B111" s="28"/>
-      <c r="C111" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="D111" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="E111" s="1"/>
-      <c r="F111" s="1"/>
-    </row>
-    <row r="112" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="30"/>
-      <c r="B112" s="28"/>
-      <c r="C112" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="E112" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="F112" s="1"/>
-    </row>
-    <row r="113" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="C112" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
         <v>218</v>
       </c>
@@ -4371,68 +4372,66 @@
         <v>218</v>
       </c>
       <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
+      <c r="E113" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="F113" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A114" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="B114" s="1" t="s">
         <v>221</v>
       </c>
+    </row>
+    <row r="114" spans="1:7" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="26" t="s">
+        <v>526</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>222</v>
+      </c>
       <c r="C114" s="26" t="s">
-        <v>220</v>
+        <v>526</v>
       </c>
       <c r="D114" s="1"/>
-      <c r="E114" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F114" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G114" s="1" t="s">
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+    </row>
+    <row r="115" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="29" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="26" t="s">
-        <v>529</v>
-      </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="C115" s="26" t="s">
-        <v>529</v>
-      </c>
-      <c r="D115" s="1"/>
+      <c r="C115" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="B116" s="28" t="s">
+    <row r="116" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A116" s="29"/>
+      <c r="B116" s="29"/>
+      <c r="C116" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="C116" s="15" t="s">
+      <c r="D116" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D116" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="E116" s="1"/>
-      <c r="F116" s="1"/>
-    </row>
-    <row r="117" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="28"/>
-      <c r="B117" s="28"/>
+      <c r="F116" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G116" s="16" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="29"/>
+      <c r="B117" s="29"/>
       <c r="C117" s="15" t="s">
         <v>228</v>
       </c>
@@ -4440,213 +4439,213 @@
         <v>229</v>
       </c>
       <c r="E117" s="1"/>
-      <c r="F117" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="G117" s="16" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="28"/>
-      <c r="B118" s="28"/>
+      <c r="F117" s="1"/>
+    </row>
+    <row r="118" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A118" s="29"/>
+      <c r="B118" s="29"/>
       <c r="C118" s="15" t="s">
         <v>230</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E118" s="1"/>
-      <c r="F118" s="1"/>
-    </row>
-    <row r="119" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A119" s="28"/>
-      <c r="B119" s="28"/>
+      <c r="E118" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G118" s="16" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="29"/>
+      <c r="B119" s="29"/>
       <c r="C119" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="D119" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="G119" s="16" t="s">
-        <v>385</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="D119" s="1"/>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="28"/>
-      <c r="B120" s="28"/>
+      <c r="A120" s="29"/>
+      <c r="B120" s="29"/>
       <c r="C120" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="D120" s="1"/>
+        <v>312</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="28"/>
-      <c r="B121" s="28"/>
-      <c r="C121" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
-    </row>
-    <row r="122" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A122" s="15" t="s">
+    <row r="121" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A121" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C121" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="D121" s="1"/>
+      <c r="E121" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="F121" s="22" t="s">
+        <v>389</v>
+      </c>
+      <c r="G121" s="16" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="C122" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1" t="s">
+      <c r="B122" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="F122" s="22" t="s">
-        <v>392</v>
-      </c>
-      <c r="G122" s="16" t="s">
+      <c r="C122" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="B123" s="28" t="s">
-        <v>239</v>
-      </c>
+      <c r="G122" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A123" s="29"/>
+      <c r="B123" s="29"/>
       <c r="C123" s="15" t="s">
         <v>240</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E123" s="1"/>
       <c r="F123" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="G123" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A124" s="28"/>
-      <c r="B124" s="28"/>
+        <v>378</v>
+      </c>
+      <c r="G123" s="16" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="29"/>
+      <c r="B124" s="29"/>
       <c r="C124" s="15" t="s">
         <v>242</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F124" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="G124" s="16" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A125" s="28"/>
-      <c r="B125" s="28"/>
-      <c r="C125" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>245</v>
-      </c>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+    </row>
+    <row r="125" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C125" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
     </row>
     <row r="126" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C126" s="26" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
-        <v>342</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>340</v>
+        <v>244</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="C127" s="26" t="s">
-        <v>342</v>
+        <v>244</v>
       </c>
       <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
-      <c r="F127" s="1"/>
-    </row>
-    <row r="128" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="E127" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F127" s="22" t="s">
+        <v>387</v>
+      </c>
+      <c r="G127" s="16" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>246</v>
+        <v>525</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>247</v>
       </c>
       <c r="C128" s="26" t="s">
-        <v>246</v>
+        <v>525</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
         <v>248</v>
       </c>
       <c r="F128" s="22" t="s">
-        <v>390</v>
-      </c>
-      <c r="G128" s="16" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A129" s="15" t="s">
-        <v>528</v>
-      </c>
-      <c r="B129" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="C129" s="26" t="s">
-        <v>528</v>
-      </c>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1" t="s">
+      <c r="B129" s="29" t="s">
         <v>250</v>
       </c>
-      <c r="F129" s="22" t="s">
-        <v>390</v>
-      </c>
-      <c r="G129" s="1" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="28" t="s">
+      <c r="C129" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="B130" s="28" t="s">
+      <c r="D129" s="1" t="s">
         <v>252</v>
       </c>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G129" s="16" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A130" s="29"/>
+      <c r="B130" s="29"/>
       <c r="C130" s="15" t="s">
         <v>253</v>
       </c>
@@ -4655,225 +4654,198 @@
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G130" s="16" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A131" s="28"/>
-      <c r="B131" s="28"/>
-      <c r="C131" s="15" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A131" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B131" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D131" s="1" t="s">
-        <v>256</v>
-      </c>
+      <c r="C131" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="D131" s="1"/>
       <c r="E131" s="1"/>
-      <c r="F131" s="1" t="s">
-        <v>377</v>
+      <c r="F131" s="22" t="s">
+        <v>385</v>
       </c>
       <c r="G131" s="16" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="28"/>
-      <c r="B132" s="28"/>
-      <c r="C132" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="D132" s="1"/>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="B132" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="C132" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="D132" s="11" t="s">
+        <v>266</v>
+      </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A133" s="15" t="s">
-        <v>526</v>
-      </c>
-      <c r="B133" s="1" t="s">
+    <row r="133" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="29"/>
+      <c r="B133" s="29"/>
+      <c r="C133" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+    </row>
+    <row r="134" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="29"/>
+      <c r="B134" s="29"/>
+      <c r="C134" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="D134" s="11" t="s">
+        <v>320</v>
+      </c>
+      <c r="E134" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="F134" s="1"/>
+    </row>
+    <row r="135" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="29"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="D135" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="E135" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="F135" s="1"/>
+    </row>
+    <row r="136" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="34" t="s">
         <v>258</v>
       </c>
-      <c r="C133" s="26" t="s">
-        <v>526</v>
-      </c>
-      <c r="D133" s="1"/>
-      <c r="E133" s="1"/>
-      <c r="F133" s="22" t="s">
-        <v>388</v>
-      </c>
-      <c r="G133" s="16" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="28" t="s">
-        <v>266</v>
-      </c>
-      <c r="B134" s="28" t="s">
+      <c r="B136" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="C136" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="C134" s="20" t="s">
+      <c r="D136" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="D134" s="11" t="s">
+      <c r="E136" s="1"/>
+      <c r="F136" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="34"/>
+      <c r="B137" s="29"/>
+      <c r="C137" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="G137" s="15" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="34"/>
+      <c r="B138" s="29"/>
+      <c r="C138" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="E134" s="1"/>
-      <c r="F134" s="1"/>
-    </row>
-    <row r="135" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="28"/>
-      <c r="B135" s="28"/>
-      <c r="C135" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="D135" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="E135" s="1"/>
-      <c r="F135" s="1"/>
-    </row>
-    <row r="136" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="28"/>
-      <c r="B136" s="28"/>
-      <c r="C136" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="D136" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="E136" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="F136" s="1"/>
-    </row>
-    <row r="137" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="28"/>
-      <c r="B137" s="28"/>
-      <c r="C137" s="15" t="s">
-        <v>334</v>
-      </c>
-      <c r="D137" s="13" t="s">
-        <v>335</v>
-      </c>
-      <c r="E137" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="F137" s="1"/>
-    </row>
-    <row r="138" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="30" t="s">
-        <v>261</v>
-      </c>
-      <c r="B138" s="28" t="s">
+      <c r="D138" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="G138" s="22" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="26" t="s">
+        <v>524</v>
+      </c>
+      <c r="B139" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="C138" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="E138" s="1"/>
-      <c r="F138" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="G138" s="1" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="30"/>
-      <c r="B139" s="28"/>
-      <c r="C139" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="G139" s="15" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="30"/>
-      <c r="B140" s="28"/>
-      <c r="C140" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="D140" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="G140" s="22" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="26" t="s">
-        <v>527</v>
-      </c>
-      <c r="B141" s="1" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A80:A83"/>
-    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="A136:A138"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="A115:A120"/>
+    <mergeCell ref="B115:B120"/>
+    <mergeCell ref="A104:A107"/>
+    <mergeCell ref="B104:B107"/>
+    <mergeCell ref="A109:A111"/>
+    <mergeCell ref="B109:B111"/>
+    <mergeCell ref="A132:A135"/>
+    <mergeCell ref="B132:B135"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="A98:A100"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="A122:A124"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="B83:B90"/>
+    <mergeCell ref="A83:A90"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="B50:B56"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B76:B77"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A8:A19"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="A43:A49"/>
-    <mergeCell ref="B84:B91"/>
-    <mergeCell ref="A84:A91"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A26:A38"/>
-    <mergeCell ref="B26:B38"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="B43:B49"/>
-    <mergeCell ref="A51:A57"/>
-    <mergeCell ref="B51:B57"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A123:A125"/>
-    <mergeCell ref="B123:B125"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="A138:A140"/>
-    <mergeCell ref="B138:B140"/>
-    <mergeCell ref="A130:A132"/>
-    <mergeCell ref="B130:B132"/>
-    <mergeCell ref="A116:A121"/>
-    <mergeCell ref="B116:B121"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="A134:A137"/>
-    <mergeCell ref="B134:B137"/>
-    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4881,15 +4853,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -5073,6 +5036,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -5080,14 +5052,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5280F00-08C5-4424-8C69-5F59D5F29D10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5101,6 +5065,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed problem with compare cycle time
Previously it existed the operation "Comparative of throughput", which was wrong due to it used a noun instead of a verb to specify the action. Now it has been fixed, since now it is "Compare throughput"
</commit_message>
<xml_diff>
--- a/OperationCoding.xlsx
+++ b/OperationCoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlo\Documents\Trabajo\BPI Challenge\bpi-challenge-performance-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23752655-8A16-415B-AD8F-4EAF73CEBA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA0324F-E9B1-4DD1-8805-17443C38DFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -444,9 +444,6 @@
     <t>It consists of determining the average, maximum, medium or minimum of how many activities, traces, or events occur for a certain unit time (for example, average trace per hour).</t>
   </si>
   <si>
-    <t>Comparative of throughput</t>
-  </si>
-  <si>
     <t>It consists of comparing the throughput for several sets of traces</t>
   </si>
   <si>
@@ -1847,6 +1844,9 @@
   </si>
   <si>
     <t>It consists of grouping events depending on the values of attributes</t>
+  </si>
+  <si>
+    <t>Compare throughput</t>
   </si>
 </sst>
 </file>
@@ -1944,7 +1944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2029,22 +2029,25 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2387,8 +2390,8 @@
   <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,16 +2407,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>512</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>514</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>513</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>515</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>516</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>0</v>
@@ -2426,11 +2429,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>512</v>
+      <c r="B2" s="30" t="s">
+        <v>511</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>4</v>
@@ -2440,32 +2443,32 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="G3" s="15" t="s">
-        <v>343</v>
-      </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="29"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
@@ -2474,15 +2477,15 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
@@ -2493,29 +2496,29 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>410</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>414</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -2531,17 +2534,17 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>412</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>413</v>
-      </c>
     </row>
     <row r="8" spans="1:7" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="30" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="15" t="s">
@@ -2552,15 +2555,15 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>344</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>345</v>
-      </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="15" t="s">
         <v>18</v>
       </c>
@@ -2573,8 +2576,8 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
@@ -2583,32 +2586,32 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>347</v>
-      </c>
     </row>
     <row r="11" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>279</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>280</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>349</v>
-      </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="15" t="s">
         <v>23</v>
       </c>
@@ -2617,32 +2620,32 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="G12" s="15" t="s">
-        <v>352</v>
-      </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="G13" s="16" t="s">
         <v>416</v>
       </c>
-      <c r="G13" s="16" t="s">
-        <v>417</v>
-      </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="15" t="s">
         <v>26</v>
       </c>
@@ -2651,32 +2654,32 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G15" s="16" t="s">
         <v>430</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>431</v>
-      </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
@@ -2685,80 +2688,80 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G16" s="16" t="s">
         <v>432</v>
       </c>
-      <c r="G16" s="16" t="s">
-        <v>433</v>
-      </c>
     </row>
     <row r="17" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="G17" s="16" t="s">
         <v>434</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>435</v>
-      </c>
     </row>
     <row r="18" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="22" t="s">
+        <v>436</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>437</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>438</v>
-      </c>
     </row>
     <row r="19" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="9"/>
       <c r="C19" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>305</v>
-      </c>
       <c r="C20" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="G20" s="16" t="s">
         <v>460</v>
-      </c>
-      <c r="G20" s="16" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2774,10 +2777,10 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="22" t="s">
+        <v>461</v>
+      </c>
+      <c r="G21" s="16" t="s">
         <v>462</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2793,10 +2796,10 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="23" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2812,10 +2815,10 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="G23" s="16" t="s">
         <v>464</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2831,10 +2834,10 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="G24" s="16" t="s">
         <v>466</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -2850,17 +2853,17 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="22" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="30" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -2871,30 +2874,30 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>384</v>
-      </c>
     </row>
     <row r="27" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="15" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>384</v>
-      </c>
     </row>
     <row r="28" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="15" t="s">
         <v>48</v>
       </c>
@@ -2903,15 +2906,15 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>398</v>
-      </c>
     </row>
     <row r="29" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="30"/>
       <c r="C29" s="15" t="s">
         <v>50</v>
       </c>
@@ -2920,15 +2923,15 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="30"/>
       <c r="C30" s="15" t="s">
         <v>52</v>
       </c>
@@ -2937,15 +2940,15 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="30"/>
       <c r="C31" s="15" t="s">
         <v>54</v>
       </c>
@@ -2954,15 +2957,15 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>421</v>
-      </c>
     </row>
     <row r="32" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
+      <c r="A32" s="30"/>
+      <c r="B32" s="30"/>
       <c r="C32" s="15" t="s">
         <v>56</v>
       </c>
@@ -2971,15 +2974,15 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>392</v>
-      </c>
     </row>
     <row r="33" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
       <c r="C33" s="15" t="s">
         <v>58</v>
       </c>
@@ -2988,15 +2991,15 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>392</v>
-      </c>
     </row>
     <row r="34" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
       <c r="C34" s="15" t="s">
         <v>60</v>
       </c>
@@ -3005,15 +3008,15 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>400</v>
-      </c>
     </row>
     <row r="35" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="15" t="s">
         <v>62</v>
       </c>
@@ -3022,15 +3025,15 @@
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="15" t="s">
         <v>64</v>
       </c>
@@ -3039,15 +3042,15 @@
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
+      <c r="A37" s="30"/>
+      <c r="B37" s="30"/>
       <c r="C37" s="15" t="s">
         <v>66</v>
       </c>
@@ -3056,38 +3059,38 @@
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="30" t="s">
         <v>69</v>
       </c>
       <c r="C38" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="D38" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="F38" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>428</v>
       </c>
-      <c r="G38" s="1" t="s">
-        <v>429</v>
-      </c>
     </row>
     <row r="39" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
+      <c r="A39" s="30"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="15" t="s">
         <v>70</v>
       </c>
@@ -3095,32 +3098,32 @@
         <v>71</v>
       </c>
       <c r="F39" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>427</v>
-      </c>
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="15" t="s">
         <v>72</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="15" t="s">
         <v>73</v>
       </c>
@@ -3131,14 +3134,14 @@
         <v>75</v>
       </c>
       <c r="F41" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="G41" s="1" t="s">
-        <v>440</v>
-      </c>
     </row>
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B42" s="33" t="s">
@@ -3152,14 +3155,14 @@
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>442</v>
-      </c>
     </row>
     <row r="43" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="33"/>
       <c r="C43" s="15" t="s">
         <v>80</v>
@@ -3171,14 +3174,14 @@
         <v>82</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="33"/>
       <c r="C44" s="15" t="s">
         <v>83</v>
@@ -3190,7 +3193,7 @@
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="33"/>
       <c r="C45" s="15" t="s">
         <v>85</v>
@@ -3200,14 +3203,14 @@
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>446</v>
-      </c>
     </row>
     <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="33"/>
       <c r="C46" s="15" t="s">
         <v>87</v>
@@ -3217,14 +3220,14 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="33"/>
       <c r="C47" s="15" t="s">
         <v>89</v>
@@ -3234,14 +3237,14 @@
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="G47" s="1" t="s">
-        <v>450</v>
-      </c>
     </row>
     <row r="48" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
+      <c r="A48" s="30"/>
       <c r="B48" s="33"/>
       <c r="C48" s="15" t="s">
         <v>91</v>
@@ -3253,10 +3256,10 @@
         <v>93</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3272,17 +3275,17 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="30" t="s">
         <v>97</v>
       </c>
       <c r="C50" s="15" t="s">
@@ -3295,15 +3298,15 @@
         <v>100</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="G50" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="G50" s="15" t="s">
-        <v>365</v>
-      </c>
     </row>
     <row r="51" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A51" s="29"/>
-      <c r="B51" s="29"/>
+      <c r="A51" s="30"/>
+      <c r="B51" s="30"/>
       <c r="C51" s="15" t="s">
         <v>101</v>
       </c>
@@ -3314,15 +3317,15 @@
         <v>103</v>
       </c>
       <c r="F51" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G51" s="16" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
-      <c r="B52" s="29"/>
+      <c r="A52" s="30"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="15" t="s">
         <v>104</v>
       </c>
@@ -3331,15 +3334,15 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="G52" s="1" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
-      <c r="B53" s="29"/>
+      <c r="A53" s="30"/>
+      <c r="B53" s="30"/>
       <c r="C53" s="15" t="s">
         <v>106</v>
       </c>
@@ -3350,15 +3353,15 @@
         <v>108</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A54" s="29"/>
-      <c r="B54" s="29"/>
+      <c r="A54" s="30"/>
+      <c r="B54" s="30"/>
       <c r="C54" s="15" t="s">
         <v>109</v>
       </c>
@@ -3369,15 +3372,15 @@
         <v>111</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G54" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="29"/>
-      <c r="B55" s="29"/>
+      <c r="A55" s="30"/>
+      <c r="B55" s="30"/>
       <c r="C55" s="15" t="s">
         <v>112</v>
       </c>
@@ -3388,15 +3391,15 @@
         <v>114</v>
       </c>
       <c r="F55" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="G55" s="16" t="s">
         <v>451</v>
       </c>
-      <c r="G55" s="16" t="s">
-        <v>452</v>
-      </c>
     </row>
     <row r="56" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
-      <c r="B56" s="29"/>
+      <c r="A56" s="30"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="15" t="s">
         <v>115</v>
       </c>
@@ -3407,17 +3410,17 @@
         <v>117</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="30" t="s">
         <v>119</v>
       </c>
       <c r="C57" s="15" t="s">
@@ -3428,32 +3431,32 @@
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G57" s="16" t="s">
         <v>454</v>
       </c>
-      <c r="G57" s="16" t="s">
-        <v>455</v>
-      </c>
     </row>
     <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
-      <c r="B58" s="29"/>
+      <c r="A58" s="30"/>
+      <c r="B58" s="30"/>
       <c r="C58" s="15" t="s">
         <v>122</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
-      <c r="B59" s="29"/>
+      <c r="A59" s="30"/>
+      <c r="B59" s="30"/>
       <c r="C59" s="15" t="s">
         <v>124</v>
       </c>
@@ -3462,27 +3465,27 @@
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G59" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="G59" s="16" t="s">
-        <v>360</v>
-      </c>
     </row>
     <row r="60" spans="1:7" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
-      <c r="B60" s="29"/>
+      <c r="A60" s="30"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3490,7 +3493,7 @@
         <v>126</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C61" s="26" t="s">
         <v>126</v>
@@ -3498,10 +3501,10 @@
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G61" s="16" t="s">
         <v>472</v>
-      </c>
-      <c r="G61" s="16" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -3517,10 +3520,10 @@
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="22" t="s">
+        <v>473</v>
+      </c>
+      <c r="G62" s="16" t="s">
         <v>474</v>
-      </c>
-      <c r="G62" s="16" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3536,10 +3539,10 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="G63" s="16" t="s">
         <v>476</v>
-      </c>
-      <c r="G63" s="16" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -3555,546 +3558,546 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="22" t="s">
+        <v>477</v>
+      </c>
+      <c r="G64" s="16" t="s">
         <v>478</v>
       </c>
-      <c r="G64" s="16" t="s">
-        <v>479</v>
-      </c>
     </row>
     <row r="65" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="29" t="s">
+        <v>527</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B65" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="C65" s="26" t="s">
-        <v>133</v>
+      <c r="C65" s="29" t="s">
+        <v>527</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F65" s="22" t="s">
+        <v>479</v>
+      </c>
+      <c r="G65" s="16" t="s">
         <v>480</v>
-      </c>
-      <c r="G65" s="16" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="C66" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="G66" s="16" t="s">
         <v>482</v>
-      </c>
-      <c r="G66" s="16" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C67" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="22" t="s">
+        <v>483</v>
+      </c>
+      <c r="G67" s="16" t="s">
         <v>484</v>
-      </c>
-      <c r="G67" s="16" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="C68" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="22" t="s">
+        <v>485</v>
+      </c>
+      <c r="G68" s="16" t="s">
         <v>486</v>
-      </c>
-      <c r="G68" s="16" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A69" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="C69" s="26" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="22" t="s">
+        <v>487</v>
+      </c>
+      <c r="G69" s="16" t="s">
         <v>488</v>
-      </c>
-      <c r="G69" s="16" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="C70" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G70" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B71" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="B71" s="16" t="s">
-        <v>146</v>
-      </c>
       <c r="C71" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="22" t="s">
+        <v>490</v>
+      </c>
+      <c r="G71" s="16" t="s">
         <v>491</v>
       </c>
-      <c r="G71" s="16" t="s">
-        <v>492</v>
-      </c>
     </row>
     <row r="72" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A72" s="29" t="s">
+      <c r="A72" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="B72" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="B72" s="29" t="s">
+      <c r="C72" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="D72" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G72" s="16" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
-      <c r="B73" s="29"/>
+      <c r="A73" s="30"/>
+      <c r="B73" s="30"/>
       <c r="C73" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D73" s="16" t="s">
         <v>151</v>
-      </c>
-      <c r="D73" s="16" t="s">
-        <v>152</v>
       </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="G73" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="G73" s="16" t="s">
+    </row>
+    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A74" s="30"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D74" s="16" t="s">
         <v>494</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A74" s="29"/>
-      <c r="B74" s="29"/>
-      <c r="C74" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="D74" s="16" t="s">
-        <v>495</v>
       </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="G74" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="G74" s="16" t="s">
+    </row>
+    <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A75" s="30"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="G75" s="16" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A75" s="29"/>
-      <c r="B75" s="29"/>
-      <c r="C75" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="G75" s="16" t="s">
-        <v>498</v>
-      </c>
-    </row>
     <row r="76" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A76" s="29" t="s">
+      <c r="A76" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="B76" s="31" t="s">
         <v>295</v>
       </c>
-      <c r="B76" s="30" t="s">
+      <c r="C76" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="D76" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>297</v>
       </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="G76" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="G76" s="17" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="77" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A77" s="29"/>
-      <c r="B77" s="30"/>
+      <c r="A77" s="30"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="D77" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>303</v>
       </c>
       <c r="E77" s="1"/>
       <c r="F77" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="C78" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="G78" s="17" t="s">
         <v>502</v>
       </c>
-      <c r="G78" s="17" t="s">
-        <v>503</v>
-      </c>
     </row>
     <row r="79" spans="1:7" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="29" t="s">
+      <c r="A79" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B79" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="B79" s="29" t="s">
+      <c r="C79" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="D79" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G79" s="1" t="s">
         <v>504</v>
       </c>
-      <c r="G79" s="1" t="s">
+    </row>
+    <row r="80" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A80" s="30"/>
+      <c r="B80" s="30"/>
+      <c r="C80" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A80" s="29"/>
-      <c r="B80" s="29"/>
-      <c r="C80" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="D80" s="4" t="s">
+      <c r="G80" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A81" s="30"/>
+      <c r="B81" s="30"/>
+      <c r="C81" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A81" s="29"/>
-      <c r="B81" s="29"/>
-      <c r="C81" s="15" t="s">
+      <c r="D81" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>166</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A82" s="29"/>
-      <c r="B82" s="29"/>
+      <c r="A82" s="30"/>
+      <c r="B82" s="30"/>
       <c r="C82" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="29" t="s">
+      <c r="A83" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B83" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="B83" s="29" t="s">
+      <c r="C83" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="C83" s="15" t="s">
+      <c r="D83" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="195" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
-      <c r="B84" s="29"/>
-      <c r="C84" s="29" t="s">
+      <c r="A84" s="30"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="D84" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="D84" s="30" t="s">
+      <c r="E84" s="31"/>
+      <c r="F84" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A85" s="30"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="31"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A86" s="30"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="E84" s="30"/>
-      <c r="F84" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A85" s="29"/>
-      <c r="B85" s="29"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="30"/>
-      <c r="E85" s="30"/>
-      <c r="F85" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A86" s="29"/>
-      <c r="B86" s="29"/>
-      <c r="C86" s="15" t="s">
+      <c r="D86" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E86" s="1"/>
       <c r="F86" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="29"/>
-      <c r="B87" s="29"/>
+      <c r="A87" s="30"/>
+      <c r="B87" s="30"/>
       <c r="C87" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
     </row>
     <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A88" s="29"/>
-      <c r="B88" s="29"/>
+      <c r="A88" s="30"/>
+      <c r="B88" s="30"/>
       <c r="C88" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="29"/>
-      <c r="B89" s="29"/>
+      <c r="A89" s="30"/>
+      <c r="B89" s="30"/>
       <c r="C89" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
-      <c r="B90" s="29"/>
+      <c r="A90" s="30"/>
+      <c r="B90" s="30"/>
       <c r="C90" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>310</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
     </row>
     <row r="91" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A91" s="29" t="s">
+      <c r="A91" s="30" t="s">
+        <v>516</v>
+      </c>
+      <c r="B91" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="C91" s="15" t="s">
         <v>517</v>
       </c>
-      <c r="B91" s="29" t="s">
+      <c r="D91" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>518</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="E91" s="1"/>
       <c r="F91" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="G91" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="G91" s="1" t="s">
-        <v>396</v>
-      </c>
     </row>
     <row r="92" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A92" s="29"/>
-      <c r="B92" s="29"/>
+      <c r="A92" s="30"/>
+      <c r="B92" s="30"/>
       <c r="C92" s="15" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
     </row>
     <row r="93" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
-      <c r="B93" s="29"/>
+      <c r="A93" s="30"/>
+      <c r="B93" s="30"/>
       <c r="C93" s="15" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
     </row>
     <row r="94" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A94" s="29"/>
-      <c r="B94" s="29"/>
+      <c r="A94" s="30"/>
+      <c r="B94" s="30"/>
       <c r="C94" s="15" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A95" s="29"/>
-      <c r="B95" s="29"/>
+      <c r="A95" s="30"/>
+      <c r="B95" s="30"/>
       <c r="C95" s="15" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="B96" s="8" t="s">
-        <v>307</v>
-      </c>
       <c r="C96" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -4102,260 +4105,260 @@
     </row>
     <row r="97" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B97" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="C97" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
     </row>
     <row r="98" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A98" s="29" t="s">
+      <c r="A98" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="B98" s="29" t="s">
+      <c r="C98" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C98" s="15" t="s">
+      <c r="D98" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D98" s="1" t="s">
+      <c r="E98" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="F98" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A99" s="30"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="F98" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A99" s="29"/>
-      <c r="B99" s="29"/>
-      <c r="C99" s="15" t="s">
+      <c r="D99" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="G99" s="1" t="s">
+    </row>
+    <row r="100" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A100" s="30"/>
+      <c r="B100" s="30"/>
+      <c r="C100" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F100" s="1" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
-      <c r="B100" s="29"/>
-      <c r="C100" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E100" s="1" t="s">
+      <c r="G100" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A101" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A101" s="29" t="s">
+      <c r="B101" s="30"/>
+      <c r="C101" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="B101" s="29"/>
-      <c r="C101" s="21" t="s">
+      <c r="D101" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D101" s="1" t="s">
+      <c r="E101" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="F101" s="1"/>
+    </row>
+    <row r="102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="30"/>
+      <c r="B102" s="30"/>
+      <c r="C102" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="F101" s="1"/>
-    </row>
-    <row r="102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="29"/>
-      <c r="B102" s="29"/>
-      <c r="C102" s="21" t="s">
+      <c r="D102" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
     <row r="103" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B103" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C103" s="26" t="s">
         <v>277</v>
-      </c>
-      <c r="C103" s="26" t="s">
-        <v>278</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
     <row r="104" spans="1:7" s="6" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="29" t="s">
+      <c r="A104" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="B104" s="30" t="s">
         <v>284</v>
       </c>
-      <c r="B104" s="29" t="s">
-        <v>285</v>
-      </c>
       <c r="C104" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="D104" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="E104" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="F104" s="22"/>
       <c r="G104" s="16"/>
     </row>
     <row r="105" spans="1:7" s="6" customFormat="1" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="29"/>
-      <c r="B105" s="29"/>
+      <c r="A105" s="30"/>
+      <c r="B105" s="30"/>
       <c r="C105" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E105" s="4"/>
       <c r="F105" s="22"/>
       <c r="G105" s="16"/>
     </row>
     <row r="106" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="29"/>
-      <c r="B106" s="29"/>
+      <c r="A106" s="30"/>
+      <c r="B106" s="30"/>
       <c r="C106" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="D106" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="E106" s="10" t="s">
         <v>316</v>
-      </c>
-      <c r="D106" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="E106" s="10" t="s">
-        <v>317</v>
       </c>
       <c r="F106" s="22"/>
       <c r="G106" s="16"/>
     </row>
     <row r="107" spans="1:7" s="6" customFormat="1" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="29"/>
-      <c r="B107" s="29"/>
+      <c r="A107" s="30"/>
+      <c r="B107" s="30"/>
       <c r="C107" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="D107" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="D107" s="10" t="s">
+      <c r="E107" s="10" t="s">
         <v>323</v>
-      </c>
-      <c r="E107" s="10" t="s">
-        <v>324</v>
       </c>
       <c r="F107" s="22"/>
       <c r="G107" s="16"/>
     </row>
     <row r="108" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B108" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="C108" s="26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D108" s="1"/>
       <c r="E108" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F108" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="F108" s="22" t="s">
+      <c r="G108" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="G108" s="1" t="s">
+    </row>
+    <row r="109" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A109" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="B109" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="C109" s="15" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A109" s="34" t="s">
-        <v>292</v>
-      </c>
-      <c r="B109" s="29" t="s">
+      <c r="D109" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F109" s="1"/>
+    </row>
+    <row r="110" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="32"/>
+      <c r="B110" s="30"/>
+      <c r="C110" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="D110" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D109" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="E109" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="F109" s="1"/>
-    </row>
-    <row r="110" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="34"/>
-      <c r="B110" s="29"/>
-      <c r="C110" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="D110" s="5" t="s">
-        <v>294</v>
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
     </row>
     <row r="111" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="34"/>
-      <c r="B111" s="29"/>
+      <c r="A111" s="32"/>
+      <c r="B111" s="30"/>
       <c r="C111" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="D111" s="9" t="s">
         <v>326</v>
       </c>
-      <c r="D111" s="9" t="s">
+      <c r="E111" s="10" t="s">
         <v>327</v>
-      </c>
-      <c r="E111" s="10" t="s">
-        <v>328</v>
       </c>
       <c r="F111" s="1"/>
     </row>
     <row r="112" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A112" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B112" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="C112" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>47</v>
@@ -4363,204 +4366,204 @@
     </row>
     <row r="113" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B113" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="C113" s="26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D113" s="1"/>
       <c r="E113" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G113" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="F113" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="26" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C114" s="26" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
     </row>
     <row r="115" spans="1:7" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="29" t="s">
+      <c r="A115" s="30" t="s">
+        <v>222</v>
+      </c>
+      <c r="B115" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="B115" s="29" t="s">
+      <c r="C115" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="C115" s="15" t="s">
-        <v>225</v>
-      </c>
       <c r="D115" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
     </row>
     <row r="116" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A116" s="29"/>
-      <c r="B116" s="29"/>
+      <c r="A116" s="30"/>
+      <c r="B116" s="30"/>
       <c r="C116" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D116" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G116" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A117" s="29"/>
-      <c r="B117" s="29"/>
+      <c r="A117" s="30"/>
+      <c r="B117" s="30"/>
       <c r="C117" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="D117" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
     </row>
     <row r="118" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A118" s="29"/>
-      <c r="B118" s="29"/>
+      <c r="A118" s="30"/>
+      <c r="B118" s="30"/>
       <c r="C118" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="D118" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D118" s="1" t="s">
+      <c r="E118" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E118" s="1" t="s">
-        <v>232</v>
-      </c>
       <c r="F118" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G118" s="16" t="s">
         <v>381</v>
       </c>
-      <c r="G118" s="16" t="s">
-        <v>382</v>
-      </c>
     </row>
     <row r="119" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="29"/>
-      <c r="B119" s="29"/>
+      <c r="A119" s="30"/>
+      <c r="B119" s="30"/>
       <c r="C119" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
     </row>
     <row r="120" spans="1:7" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="29"/>
-      <c r="B120" s="29"/>
+      <c r="A120" s="30"/>
+      <c r="B120" s="30"/>
       <c r="C120" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="D120" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
     </row>
     <row r="121" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A121" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B121" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B121" s="1" t="s">
-        <v>234</v>
-      </c>
       <c r="C121" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D121" s="1"/>
       <c r="E121" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F121" s="22" t="s">
+        <v>388</v>
+      </c>
+      <c r="G121" s="16" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="F121" s="22" t="s">
-        <v>389</v>
-      </c>
-      <c r="G121" s="16" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="29" t="s">
+      <c r="B122" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="B122" s="29" t="s">
+      <c r="C122" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="C122" s="15" t="s">
+      <c r="D122" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="E122" s="1"/>
       <c r="F122" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="G122" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="G122" s="1" t="s">
-        <v>394</v>
-      </c>
     </row>
     <row r="123" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A123" s="29"/>
-      <c r="B123" s="29"/>
+      <c r="A123" s="30"/>
+      <c r="B123" s="30"/>
       <c r="C123" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="F123" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G123" s="16" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A124" s="30"/>
+      <c r="B124" s="30"/>
+      <c r="C124" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="G123" s="16" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A124" s="29"/>
-      <c r="B124" s="29"/>
-      <c r="C124" s="15" t="s">
+      <c r="D124" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
     </row>
     <row r="125" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="B125" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="B125" s="9" t="s">
-        <v>330</v>
-      </c>
       <c r="C125" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -4568,13 +4571,13 @@
     </row>
     <row r="126" spans="1:7" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C126" s="26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
@@ -4582,230 +4585,245 @@
     </row>
     <row r="127" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A127" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B127" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B127" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="C127" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D127" s="1"/>
       <c r="E127" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F127" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="G127" s="16" t="s">
         <v>387</v>
-      </c>
-      <c r="G127" s="16" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C128" s="26" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F128" s="22" t="s">
+        <v>386</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="F128" s="22" t="s">
-        <v>387</v>
-      </c>
-      <c r="G128" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="29" t="s">
+      <c r="B129" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="B129" s="29" t="s">
+      <c r="C129" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C129" s="15" t="s">
+      <c r="D129" s="1" t="s">
         <v>251</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G129" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="G129" s="16" t="s">
-        <v>375</v>
-      </c>
     </row>
     <row r="130" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A130" s="29"/>
-      <c r="B130" s="29"/>
+      <c r="A130" s="30"/>
+      <c r="B130" s="30"/>
       <c r="C130" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G130" s="16" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A131" s="15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C131" s="26" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="G131" s="16" t="s">
         <v>385</v>
       </c>
-      <c r="G131" s="16" t="s">
-        <v>386</v>
-      </c>
     </row>
     <row r="132" spans="1:7" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="29" t="s">
+      <c r="A132" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="B132" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="B132" s="29" t="s">
+      <c r="C132" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="C132" s="20" t="s">
+      <c r="D132" s="11" t="s">
         <v>265</v>
-      </c>
-      <c r="D132" s="11" t="s">
-        <v>266</v>
       </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
     </row>
     <row r="133" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="29"/>
-      <c r="B133" s="29"/>
+      <c r="A133" s="30"/>
+      <c r="B133" s="30"/>
       <c r="C133" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="D133" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="D133" s="12" t="s">
-        <v>257</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
     </row>
     <row r="134" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="29"/>
-      <c r="B134" s="29"/>
+      <c r="A134" s="30"/>
+      <c r="B134" s="30"/>
       <c r="C134" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="D134" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="D134" s="11" t="s">
+      <c r="E134" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="E134" s="10" t="s">
-        <v>321</v>
-      </c>
       <c r="F134" s="1"/>
     </row>
     <row r="135" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="29"/>
-      <c r="B135" s="29"/>
+      <c r="A135" s="30"/>
+      <c r="B135" s="30"/>
       <c r="C135" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="D135" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="D135" s="13" t="s">
+      <c r="E135" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="E135" s="10" t="s">
-        <v>333</v>
-      </c>
       <c r="F135" s="1"/>
     </row>
     <row r="136" spans="1:7" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="34" t="s">
+      <c r="A136" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="B136" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="B136" s="29" t="s">
-        <v>259</v>
-      </c>
       <c r="C136" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="D136" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="E136" s="1"/>
       <c r="F136" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G136" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="32"/>
+      <c r="B137" s="30"/>
+      <c r="C137" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F137" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G137" s="15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="32"/>
+      <c r="B138" s="30"/>
+      <c r="C138" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="G138" s="22" t="s">
         <v>407</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
-      <c r="B137" s="29"/>
-      <c r="C137" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="D137" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="F137" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="G137" s="15" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="34"/>
-      <c r="B138" s="29"/>
-      <c r="C138" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="D138" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="G138" s="22" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="B72:B75"/>
+    <mergeCell ref="B79:B82"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="B38:B41"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="B50:B56"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A8:A19"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A48"/>
+    <mergeCell ref="A26:A37"/>
+    <mergeCell ref="B26:B37"/>
     <mergeCell ref="A136:A138"/>
     <mergeCell ref="B136:B138"/>
     <mergeCell ref="A115:A120"/>
@@ -4816,36 +4834,21 @@
     <mergeCell ref="B109:B111"/>
     <mergeCell ref="A132:A135"/>
     <mergeCell ref="B132:B135"/>
+    <mergeCell ref="A122:A124"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="E84:E85"/>
     <mergeCell ref="A91:A95"/>
     <mergeCell ref="B91:B95"/>
     <mergeCell ref="A98:A100"/>
     <mergeCell ref="B98:B100"/>
     <mergeCell ref="B101:B102"/>
-    <mergeCell ref="A122:A124"/>
-    <mergeCell ref="B122:B124"/>
     <mergeCell ref="A101:A102"/>
     <mergeCell ref="B83:B90"/>
     <mergeCell ref="A83:A90"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="B38:B41"/>
-    <mergeCell ref="B42:B48"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="B50:B56"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="B72:B75"/>
-    <mergeCell ref="B79:B82"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A79:A82"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A8:A19"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A42:A48"/>
-    <mergeCell ref="A26:A37"/>
-    <mergeCell ref="B26:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4853,6 +4856,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D009037354106145AFF53138C3A15B5B" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="1192de137dfb0dac501f70ec84eca612">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49df82a0-becc-4ef3-aa57-ac77f6d841c6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="585a6fc3ef7f7fa528f2c37fd9f8cac5" ns2:_="">
     <xsd:import namespace="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
@@ -5036,22 +5054,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5280F00-08C5-4424-8C69-5F59D5F29D10}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5067,28 +5094,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DA2DC54-7D78-41CD-B776-ED94CCCAC36D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E3241CC-812D-4AE0-87E3-DC763F2B6D27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="49df82a0-becc-4ef3-aa57-ac77f6d841c6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>